<commit_message>
Updated SGW WBS Project Plan 6Dec17
</commit_message>
<xml_diff>
--- a/2017-18 SGW WBS Project Plan.xlsx
+++ b/2017-18 SGW WBS Project Plan.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="88">
   <si>
     <t>Planned Start Date</t>
   </si>
@@ -527,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -555,24 +555,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -586,11 +568,25 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -600,8 +596,15 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -921,7 +924,7 @@
       <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P48" sqref="P48"/>
+      <selection pane="bottomRight" activeCell="J71" sqref="J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
@@ -953,65 +956,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="37">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="35">
         <v>2017</v>
       </c>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="39">
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="37">
         <v>2018</v>
       </c>
-      <c r="AC1" s="24"/>
-      <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
-      <c r="AJ1" s="24"/>
-      <c r="AK1" s="24"/>
-      <c r="AL1" s="24"/>
-      <c r="AM1" s="24"/>
-      <c r="AN1" s="24"/>
-      <c r="AO1" s="24"/>
-      <c r="AP1" s="24"/>
-      <c r="AQ1" s="24"/>
-      <c r="AR1" s="40"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
+      <c r="AM1" s="38"/>
+      <c r="AN1" s="38"/>
+      <c r="AO1" s="38"/>
+      <c r="AP1" s="38"/>
+      <c r="AQ1" s="38"/>
+      <c r="AR1" s="39"/>
     </row>
     <row r="2" spans="1:58" s="7" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="27" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="21" t="s">
         <v>40</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1167,38 +1170,38 @@
       <c r="J3" s="13"/>
       <c r="K3" s="14"/>
       <c r="L3" s="15"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
-      <c r="Y3" s="36"/>
-      <c r="Z3" s="36"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="35"/>
-      <c r="AG3" s="35"/>
-      <c r="AH3" s="35"/>
-      <c r="AI3" s="35"/>
-      <c r="AJ3" s="35"/>
-      <c r="AK3" s="35"/>
-      <c r="AL3" s="35"/>
-      <c r="AM3" s="35"/>
-      <c r="AN3" s="35"/>
-      <c r="AO3" s="35"/>
-      <c r="AP3" s="35"/>
-      <c r="AQ3" s="35"/>
-      <c r="AR3" s="35"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="28"/>
+      <c r="AB3" s="28"/>
+      <c r="AC3" s="28"/>
+      <c r="AD3" s="28"/>
+      <c r="AE3" s="28"/>
+      <c r="AF3" s="28"/>
+      <c r="AG3" s="28"/>
+      <c r="AH3" s="28"/>
+      <c r="AI3" s="28"/>
+      <c r="AJ3" s="28"/>
+      <c r="AK3" s="28"/>
+      <c r="AL3" s="28"/>
+      <c r="AM3" s="28"/>
+      <c r="AN3" s="28"/>
+      <c r="AO3" s="28"/>
+      <c r="AP3" s="28"/>
+      <c r="AQ3" s="28"/>
+      <c r="AR3" s="28"/>
     </row>
     <row r="4" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -1222,7 +1225,7 @@
       <c r="I4" s="12">
         <v>43061</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="22">
         <v>1</v>
       </c>
       <c r="K4" s="19" t="s">
@@ -1280,9 +1283,7 @@
         <v>43069</v>
       </c>
       <c r="I5" s="11"/>
-      <c r="J5" s="32" t="s">
-        <v>47</v>
-      </c>
+      <c r="J5" s="40"/>
       <c r="K5" s="14"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
@@ -1708,9 +1709,7 @@
         <v>43069</v>
       </c>
       <c r="I12" s="11"/>
-      <c r="J12" s="17">
-        <v>1</v>
-      </c>
+      <c r="J12" s="41"/>
       <c r="K12" s="19" t="s">
         <v>36</v>
       </c>
@@ -1752,7 +1751,7 @@
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="27" t="s">
         <v>82</v>
       </c>
       <c r="E13" s="10">
@@ -1814,7 +1813,7 @@
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="27" t="s">
         <v>83</v>
       </c>
       <c r="E14" s="10">
@@ -1830,7 +1829,7 @@
         <v>43069</v>
       </c>
       <c r="I14" s="11"/>
-      <c r="J14" s="31" t="s">
+      <c r="J14" s="25" t="s">
         <v>47</v>
       </c>
       <c r="K14" s="19" t="s">
@@ -1899,15 +1898,15 @@
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
-      <c r="S15" s="36"/>
-      <c r="T15" s="36"/>
-      <c r="U15" s="36"/>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
-      <c r="X15" s="36"/>
-      <c r="Y15" s="36"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="29"/>
+      <c r="Y15" s="29"/>
       <c r="Z15" s="15"/>
       <c r="AA15" s="15"/>
       <c r="AB15" s="15"/>
@@ -2356,7 +2355,7 @@
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="23" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="16">
@@ -2807,7 +2806,7 @@
       <c r="J30" s="17">
         <v>1</v>
       </c>
-      <c r="K30" s="30" t="s">
+      <c r="K30" s="24" t="s">
         <v>54</v>
       </c>
       <c r="L30" s="15"/>
@@ -3217,7 +3216,7 @@
       <c r="AR36" s="15"/>
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="26" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="9"/>
@@ -3249,8 +3248,8 @@
       <c r="R37" s="15"/>
       <c r="S37" s="15"/>
       <c r="T37" s="15"/>
-      <c r="U37" s="36"/>
-      <c r="V37" s="36"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
       <c r="W37" s="15"/>
       <c r="X37" s="15"/>
       <c r="Y37" s="15"/>
@@ -3645,7 +3644,7 @@
       <c r="AR43" s="15"/>
     </row>
     <row r="44" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A44" s="33" t="s">
+      <c r="A44" s="26" t="s">
         <v>87</v>
       </c>
       <c r="B44" s="9"/>
@@ -3677,18 +3676,18 @@
       <c r="X44" s="15"/>
       <c r="Y44" s="15"/>
       <c r="Z44" s="15"/>
-      <c r="AA44" s="36"/>
-      <c r="AB44" s="36"/>
-      <c r="AC44" s="36"/>
-      <c r="AD44" s="36"/>
-      <c r="AE44" s="36"/>
-      <c r="AF44" s="36"/>
-      <c r="AG44" s="36"/>
-      <c r="AH44" s="36"/>
-      <c r="AI44" s="36"/>
-      <c r="AJ44" s="36"/>
-      <c r="AK44" s="36"/>
-      <c r="AL44" s="36"/>
+      <c r="AA44" s="29"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="29"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="29"/>
+      <c r="AF44" s="29"/>
+      <c r="AG44" s="29"/>
+      <c r="AH44" s="29"/>
+      <c r="AI44" s="29"/>
+      <c r="AJ44" s="29"/>
+      <c r="AK44" s="29"/>
+      <c r="AL44" s="29"/>
       <c r="AM44" s="15"/>
       <c r="AN44" s="15"/>
       <c r="AO44" s="15"/>
@@ -4289,7 +4288,7 @@
       <c r="AR55" s="15"/>
     </row>
     <row r="56" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A56" s="33" t="s">
+      <c r="A56" s="26" t="s">
         <v>74</v>
       </c>
       <c r="B56" s="9"/>
@@ -4336,8 +4335,8 @@
       <c r="AK56" s="15"/>
       <c r="AL56" s="15"/>
       <c r="AM56" s="15"/>
-      <c r="AN56" s="36"/>
-      <c r="AO56" s="36"/>
+      <c r="AN56" s="29"/>
+      <c r="AO56" s="29"/>
       <c r="AP56" s="15"/>
       <c r="AQ56" s="15"/>
       <c r="AR56" s="15"/>
@@ -4647,24 +4646,24 @@
       <c r="X62" s="15"/>
       <c r="Y62" s="15"/>
       <c r="Z62" s="15"/>
-      <c r="AA62" s="36"/>
-      <c r="AB62" s="36"/>
-      <c r="AC62" s="36"/>
-      <c r="AD62" s="36"/>
-      <c r="AE62" s="36"/>
-      <c r="AF62" s="36"/>
-      <c r="AG62" s="36"/>
-      <c r="AH62" s="36"/>
-      <c r="AI62" s="36"/>
-      <c r="AJ62" s="36"/>
-      <c r="AK62" s="36"/>
-      <c r="AL62" s="36"/>
-      <c r="AM62" s="36"/>
-      <c r="AN62" s="36"/>
-      <c r="AO62" s="36"/>
-      <c r="AP62" s="36"/>
-      <c r="AQ62" s="36"/>
-      <c r="AR62" s="36"/>
+      <c r="AA62" s="29"/>
+      <c r="AB62" s="29"/>
+      <c r="AC62" s="29"/>
+      <c r="AD62" s="29"/>
+      <c r="AE62" s="29"/>
+      <c r="AF62" s="29"/>
+      <c r="AG62" s="29"/>
+      <c r="AH62" s="29"/>
+      <c r="AI62" s="29"/>
+      <c r="AJ62" s="29"/>
+      <c r="AK62" s="29"/>
+      <c r="AL62" s="29"/>
+      <c r="AM62" s="29"/>
+      <c r="AN62" s="29"/>
+      <c r="AO62" s="29"/>
+      <c r="AP62" s="29"/>
+      <c r="AQ62" s="29"/>
+      <c r="AR62" s="29"/>
     </row>
     <row r="63" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
@@ -4781,16 +4780,24 @@
         <v>22</v>
       </c>
       <c r="D65" s="10"/>
-      <c r="E65" s="10"/>
+      <c r="E65" s="10">
+        <v>2</v>
+      </c>
       <c r="F65" s="11">
         <v>43073</v>
       </c>
-      <c r="G65" s="11"/>
+      <c r="G65" s="11">
+        <v>43073</v>
+      </c>
       <c r="H65" s="11">
         <v>43077</v>
       </c>
-      <c r="I65" s="12"/>
-      <c r="J65" s="13"/>
+      <c r="I65" s="11">
+        <v>43077</v>
+      </c>
+      <c r="J65" s="17">
+        <v>1</v>
+      </c>
       <c r="K65" s="19" t="s">
         <v>36</v>
       </c>
@@ -4974,7 +4981,7 @@
       <c r="S68" s="15"/>
       <c r="T68" s="15"/>
       <c r="U68" s="15"/>
-      <c r="V68" s="36"/>
+      <c r="V68" s="29"/>
       <c r="W68" s="15"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
@@ -5038,8 +5045,8 @@
       <c r="U69" s="15"/>
       <c r="V69" s="15"/>
       <c r="W69" s="15"/>
-      <c r="X69" s="36"/>
-      <c r="Y69" s="36"/>
+      <c r="X69" s="29"/>
+      <c r="Y69" s="29"/>
       <c r="Z69" s="15"/>
       <c r="AA69" s="15"/>
       <c r="AB69" s="15"/>

</xml_diff>

<commit_message>
Updated SGW WBS Project Plan 8Dec17
Updated Owners column and left pane linkages
</commit_message>
<xml_diff>
--- a/2017-18 SGW WBS Project Plan.xlsx
+++ b/2017-18 SGW WBS Project Plan.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>Planned Start Date</t>
   </si>
@@ -572,6 +572,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -601,10 +605,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,7 +906,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -924,7 +924,7 @@
       <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J71" sqref="J71"/>
+      <selection pane="bottomRight" activeCell="N71" sqref="N71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
@@ -956,64 +956,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="35">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="37">
         <v>2017</v>
       </c>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="37">
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="39">
         <v>2018</v>
       </c>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
-      <c r="AM1" s="38"/>
-      <c r="AN1" s="38"/>
-      <c r="AO1" s="38"/>
-      <c r="AP1" s="38"/>
-      <c r="AQ1" s="38"/>
-      <c r="AR1" s="39"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="40"/>
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="40"/>
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
+      <c r="AK1" s="40"/>
+      <c r="AL1" s="40"/>
+      <c r="AM1" s="40"/>
+      <c r="AN1" s="40"/>
+      <c r="AO1" s="40"/>
+      <c r="AP1" s="40"/>
+      <c r="AQ1" s="40"/>
+      <c r="AR1" s="41"/>
     </row>
     <row r="2" spans="1:58" s="7" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="21" t="s">
         <v>40</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="AQ4" s="15"/>
       <c r="AR4" s="15"/>
     </row>
-    <row r="5" spans="1:58" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
         <v>31</v>
@@ -1283,7 +1283,7 @@
         <v>43069</v>
       </c>
       <c r="I5" s="11"/>
-      <c r="J5" s="40"/>
+      <c r="J5" s="30"/>
       <c r="K5" s="14"/>
       <c r="L5" s="15"/>
       <c r="M5" s="15"/>
@@ -1319,7 +1319,7 @@
       <c r="AQ5" s="15"/>
       <c r="AR5" s="15"/>
     </row>
-    <row r="6" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
@@ -1381,7 +1381,7 @@
       <c r="AQ6" s="15"/>
       <c r="AR6" s="15"/>
     </row>
-    <row r="7" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="18" t="s">
@@ -1443,7 +1443,7 @@
       <c r="AQ7" s="15"/>
       <c r="AR7" s="15"/>
     </row>
-    <row r="8" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="18" t="s">
@@ -1505,7 +1505,7 @@
       <c r="AQ8" s="15"/>
       <c r="AR8" s="15"/>
     </row>
-    <row r="9" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="18" t="s">
@@ -1567,7 +1567,7 @@
       <c r="AQ9" s="15"/>
       <c r="AR9" s="15"/>
     </row>
-    <row r="10" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="18" t="s">
@@ -1629,7 +1629,7 @@
       <c r="AQ10" s="15"/>
       <c r="AR10" s="15"/>
     </row>
-    <row r="11" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="18" t="s">
@@ -1691,7 +1691,7 @@
       <c r="AQ11" s="15"/>
       <c r="AR11" s="15"/>
     </row>
-    <row r="12" spans="1:58" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="18" t="s">
@@ -1709,7 +1709,7 @@
         <v>43069</v>
       </c>
       <c r="I12" s="11"/>
-      <c r="J12" s="41"/>
+      <c r="J12" s="31"/>
       <c r="K12" s="19" t="s">
         <v>36</v>
       </c>
@@ -1747,7 +1747,7 @@
       <c r="AQ12" s="15"/>
       <c r="AR12" s="15"/>
     </row>
-    <row r="13" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1809,7 +1809,7 @@
       <c r="AQ13" s="15"/>
       <c r="AR13" s="15"/>
     </row>
-    <row r="14" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -2723,7 +2723,7 @@
       <c r="AQ28" s="15"/>
       <c r="AR28" s="15"/>
     </row>
-    <row r="29" spans="1:44" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="18" t="s">
         <v>48</v>
@@ -2781,7 +2781,7 @@
       <c r="AQ29" s="15"/>
       <c r="AR29" s="15"/>
     </row>
-    <row r="30" spans="1:44" ht="16.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:44" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="18" t="s">
@@ -2843,7 +2843,7 @@
       <c r="AQ30" s="15"/>
       <c r="AR30" s="15"/>
     </row>
-    <row r="31" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="18" t="s">
@@ -2967,7 +2967,7 @@
       <c r="AQ32" s="15"/>
       <c r="AR32" s="15"/>
     </row>
-    <row r="33" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="18" t="s">
@@ -3029,7 +3029,7 @@
       <c r="AQ33" s="15"/>
       <c r="AR33" s="15"/>
     </row>
-    <row r="34" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="18" t="s">
@@ -3091,7 +3091,7 @@
       <c r="AQ34" s="15"/>
       <c r="AR34" s="15"/>
     </row>
-    <row r="35" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
       <c r="C35" s="18" t="s">
@@ -4125,7 +4125,7 @@
       <c r="AQ52" s="15"/>
       <c r="AR52" s="15"/>
     </row>
-    <row r="53" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="18" t="s">
         <v>65</v>
@@ -4179,7 +4179,7 @@
       <c r="AQ53" s="15"/>
       <c r="AR53" s="15"/>
     </row>
-    <row r="54" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="18" t="s">
         <v>66</v>
@@ -4304,9 +4304,7 @@
       </c>
       <c r="I56" s="12"/>
       <c r="J56" s="13"/>
-      <c r="K56" s="19" t="s">
-        <v>70</v>
-      </c>
+      <c r="K56" s="19"/>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
@@ -4449,7 +4447,7 @@
       <c r="AQ58" s="15"/>
       <c r="AR58" s="15"/>
     </row>
-    <row r="59" spans="1:44" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="9" t="s">
         <v>24</v>
@@ -4503,7 +4501,7 @@
       <c r="AQ59" s="15"/>
       <c r="AR59" s="15"/>
     </row>
-    <row r="60" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9" t="s">
@@ -4557,7 +4555,7 @@
       <c r="AQ60" s="15"/>
       <c r="AR60" s="15"/>
     </row>
-    <row r="61" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9" t="s">
@@ -4628,9 +4626,7 @@
       </c>
       <c r="I62" s="12"/>
       <c r="J62" s="13"/>
-      <c r="K62" s="19" t="s">
-        <v>36</v>
-      </c>
+      <c r="K62" s="19"/>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
@@ -4719,7 +4715,7 @@
       <c r="AQ63" s="15"/>
       <c r="AR63" s="15"/>
     </row>
-    <row r="64" spans="1:44" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="18" t="s">
         <v>72</v>
@@ -4773,7 +4769,7 @@
       <c r="AQ64" s="15"/>
       <c r="AR64" s="15"/>
     </row>
-    <row r="65" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9" t="s">
@@ -4835,7 +4831,7 @@
       <c r="AQ65" s="15"/>
       <c r="AR65" s="15"/>
     </row>
-    <row r="66" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9" t="s">
@@ -4889,7 +4885,7 @@
       <c r="AQ66" s="15"/>
       <c r="AR66" s="15"/>
     </row>
-    <row r="67" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="9"/>
       <c r="C67" s="18" t="s">

</xml_diff>

<commit_message>
Updated WBS Project Plan 21Apr18
added duration/hours for each task
</commit_message>
<xml_diff>
--- a/2017-18 SGW WBS Project Plan.xlsx
+++ b/2017-18 SGW WBS Project Plan.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
   <si>
     <t>Planned Start Date</t>
   </si>
@@ -124,9 +124,6 @@
     <t>1.2.1  Define Scope</t>
   </si>
   <si>
-    <t>6.1  Develop User Manual/Documentation</t>
-  </si>
-  <si>
     <t>Jennifer</t>
   </si>
   <si>
@@ -208,9 +205,6 @@
     <t>3.3  Schedule test with stakeholder</t>
   </si>
   <si>
-    <t>3.4  Conduct test and record video of test</t>
-  </si>
-  <si>
     <t>Eliseo, Clark</t>
   </si>
   <si>
@@ -287,6 +281,45 @@
   </si>
   <si>
     <t>4.0  Build and Test the Site &amp; Volunteer Application</t>
+  </si>
+  <si>
+    <t>6.1  Develop User Guides and Video Tutorials</t>
+  </si>
+  <si>
+    <t>8.1  Rebuild Reports site using PHPRunner (free version)</t>
+  </si>
+  <si>
+    <t>8.2  Update site to add Section field (SGW &amp; Hardman Farm)</t>
+  </si>
+  <si>
+    <t>Eliseo, Andrea</t>
+  </si>
+  <si>
+    <t>Alex, Eliseo</t>
+  </si>
+  <si>
+    <t>Clark, Jennifer</t>
+  </si>
+  <si>
+    <t>Andrea, Jennifer</t>
+  </si>
+  <si>
+    <t>3.4  Conduct test and record test results</t>
+  </si>
+  <si>
+    <t>4.2.1  Use current WordPress to rebuild site</t>
+  </si>
+  <si>
+    <t>4.2.2  Use plugins to build Volunteer app in WP</t>
+  </si>
+  <si>
+    <t>4.2.3  Rebuild app as standalone with MySQLi</t>
+  </si>
+  <si>
+    <t>Jennifer, Eliseo</t>
+  </si>
+  <si>
+    <t>TOTAL DURATION (hr)</t>
   </si>
 </sst>
 </file>
@@ -358,7 +391,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +431,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -605,6 +644,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,7 +952,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -918,13 +964,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BF69"/>
+  <dimension ref="A1:BF75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="2" topLeftCell="AD3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N71" sqref="N71"/>
+      <selection pane="bottomRight" activeCell="AF77" sqref="AF77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
@@ -957,7 +1003,7 @@
   <sheetData>
     <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -1015,7 +1061,7 @@
       <c r="C2" s="33"/>
       <c r="D2" s="34"/>
       <c r="E2" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -1229,7 +1275,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
@@ -1345,7 +1391,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
@@ -1385,7 +1431,7 @@
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10">
@@ -1407,7 +1453,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
@@ -1447,7 +1493,7 @@
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10">
@@ -1469,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
@@ -1509,7 +1555,7 @@
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10">
@@ -1531,7 +1577,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
@@ -1571,7 +1617,7 @@
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10">
@@ -1593,7 +1639,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
@@ -1633,7 +1679,7 @@
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10">
@@ -1655,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
@@ -1695,7 +1741,7 @@
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1711,7 +1757,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="31"/>
       <c r="K12" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
@@ -1752,7 +1798,7 @@
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
@@ -1773,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
@@ -1814,7 +1860,7 @@
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E14" s="10">
         <v>2</v>
@@ -1830,10 +1876,10 @@
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
@@ -1889,9 +1935,7 @@
       <c r="I15" s="11">
         <v>43051</v>
       </c>
-      <c r="J15" s="17">
-        <v>1</v>
-      </c>
+      <c r="J15" s="43"/>
       <c r="K15" s="20"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
@@ -1947,9 +1991,7 @@
       <c r="I16" s="11">
         <v>43018</v>
       </c>
-      <c r="J16" s="17">
-        <v>1</v>
-      </c>
+      <c r="J16" s="43"/>
       <c r="K16" s="14"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
@@ -2011,7 +2053,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
@@ -2073,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
@@ -2135,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
@@ -2191,9 +2233,7 @@
       <c r="I20" s="11">
         <v>43018</v>
       </c>
-      <c r="J20" s="17">
-        <v>1</v>
-      </c>
+      <c r="J20" s="43"/>
       <c r="K20" s="14"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15"/>
@@ -2249,11 +2289,9 @@
       <c r="I21" s="11">
         <v>43018</v>
       </c>
-      <c r="J21" s="17">
-        <v>1</v>
-      </c>
+      <c r="J21" s="43"/>
       <c r="K21" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
@@ -2315,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
@@ -2356,7 +2394,7 @@
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="16">
         <v>1</v>
@@ -2377,7 +2415,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
@@ -2417,7 +2455,7 @@
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10">
@@ -2439,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
@@ -2479,7 +2517,7 @@
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10">
@@ -2501,7 +2539,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
@@ -2541,7 +2579,7 @@
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10">
@@ -2563,7 +2601,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
@@ -2603,7 +2641,7 @@
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10">
@@ -2625,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
@@ -2665,7 +2703,7 @@
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10">
@@ -2687,7 +2725,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
@@ -2726,7 +2764,7 @@
     <row r="29" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
@@ -2743,9 +2781,7 @@
       <c r="I29" s="11">
         <v>43018</v>
       </c>
-      <c r="J29" s="17">
-        <v>1</v>
-      </c>
+      <c r="J29" s="43"/>
       <c r="K29" s="14"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
@@ -2785,7 +2821,7 @@
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10">
@@ -2807,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
@@ -2847,7 +2883,7 @@
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10">
@@ -2869,7 +2905,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
@@ -2909,7 +2945,7 @@
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10">
@@ -2931,7 +2967,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
@@ -2971,7 +3007,7 @@
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10">
@@ -2993,7 +3029,7 @@
         <v>1</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
@@ -3033,7 +3069,7 @@
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10">
@@ -3055,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
@@ -3095,7 +3131,7 @@
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
       <c r="C35" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10">
@@ -3117,7 +3153,7 @@
         <v>1</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
@@ -3156,7 +3192,7 @@
     <row r="36" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="10"/>
@@ -3179,7 +3215,7 @@
         <v>1</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
@@ -3217,7 +3253,7 @@
     </row>
     <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -3235,9 +3271,7 @@
       <c r="I37" s="11">
         <v>43034</v>
       </c>
-      <c r="J37" s="17">
-        <v>1</v>
-      </c>
+      <c r="J37" s="43"/>
       <c r="K37" s="14"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
@@ -3276,7 +3310,7 @@
     <row r="38" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
@@ -3293,11 +3327,9 @@
       <c r="I38" s="11">
         <v>43033</v>
       </c>
-      <c r="J38" s="17">
-        <v>1</v>
-      </c>
+      <c r="J38" s="43"/>
       <c r="K38" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
@@ -3337,7 +3369,7 @@
       <c r="A39" s="8"/>
       <c r="B39" s="9"/>
       <c r="C39" s="18" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10">
@@ -3359,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
@@ -3399,7 +3431,7 @@
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10">
@@ -3421,7 +3453,7 @@
         <v>1</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
@@ -3460,7 +3492,7 @@
     <row r="41" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
@@ -3522,7 +3554,7 @@
     <row r="42" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
@@ -3545,7 +3577,7 @@
         <v>1</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
@@ -3584,12 +3616,12 @@
     <row r="43" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="18" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F43" s="11">
         <v>43032</v>
@@ -3607,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
@@ -3645,7 +3677,7 @@
     </row>
     <row r="44" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3654,12 +3686,16 @@
       <c r="F44" s="11">
         <v>43080</v>
       </c>
-      <c r="G44" s="11"/>
+      <c r="G44" s="11">
+        <v>43080</v>
+      </c>
       <c r="H44" s="11">
         <v>43174</v>
       </c>
-      <c r="I44" s="12"/>
-      <c r="J44" s="13"/>
+      <c r="I44" s="11">
+        <v>43174</v>
+      </c>
+      <c r="J44" s="43"/>
       <c r="K44" s="14"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
@@ -3706,15 +3742,17 @@
       <c r="F45" s="11">
         <v>43080</v>
       </c>
-      <c r="G45" s="11"/>
+      <c r="G45" s="11">
+        <v>43080</v>
+      </c>
       <c r="H45" s="11">
         <v>43084</v>
       </c>
-      <c r="I45" s="12"/>
-      <c r="J45" s="13"/>
-      <c r="K45" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="I45" s="11">
+        <v>43084</v>
+      </c>
+      <c r="J45" s="43"/>
+      <c r="K45" s="19"/>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
@@ -3756,17 +3794,27 @@
         <v>14</v>
       </c>
       <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
+      <c r="E46" s="10">
+        <v>2</v>
+      </c>
       <c r="F46" s="11">
         <v>43080</v>
       </c>
-      <c r="G46" s="11"/>
+      <c r="G46" s="11">
+        <v>43080</v>
+      </c>
       <c r="H46" s="11">
         <v>43084</v>
       </c>
-      <c r="I46" s="12"/>
-      <c r="J46" s="13"/>
-      <c r="K46" s="14"/>
+      <c r="I46" s="11">
+        <v>43084</v>
+      </c>
+      <c r="J46" s="17">
+        <v>1</v>
+      </c>
+      <c r="K46" s="14" t="s">
+        <v>91</v>
+      </c>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
@@ -3804,7 +3852,7 @@
     <row r="47" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="18" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
@@ -3812,14 +3860,18 @@
       <c r="F47" s="11">
         <v>43080</v>
       </c>
-      <c r="G47" s="11"/>
+      <c r="G47" s="11">
+        <v>43080</v>
+      </c>
       <c r="H47" s="11">
         <v>43125</v>
       </c>
-      <c r="I47" s="12"/>
-      <c r="J47" s="13"/>
+      <c r="I47" s="11">
+        <v>43125</v>
+      </c>
+      <c r="J47" s="43"/>
       <c r="K47" s="19" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
@@ -3836,11 +3888,11 @@
       <c r="X47" s="15"/>
       <c r="Y47" s="15"/>
       <c r="Z47" s="15"/>
-      <c r="AA47" s="15"/>
-      <c r="AB47" s="15"/>
-      <c r="AC47" s="15"/>
-      <c r="AD47" s="15"/>
-      <c r="AE47" s="15"/>
+      <c r="AA47" s="29"/>
+      <c r="AB47" s="29"/>
+      <c r="AC47" s="29"/>
+      <c r="AD47" s="29"/>
+      <c r="AE47" s="29"/>
       <c r="AF47" s="15"/>
       <c r="AG47" s="15"/>
       <c r="AH47" s="15"/>
@@ -3857,23 +3909,31 @@
     </row>
     <row r="48" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
-      <c r="B48" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="9"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
+      <c r="E48" s="10">
+        <v>12</v>
+      </c>
       <c r="F48" s="11">
-        <v>43126</v>
-      </c>
-      <c r="G48" s="11"/>
+        <v>43080</v>
+      </c>
+      <c r="G48" s="11">
+        <v>43080</v>
+      </c>
       <c r="H48" s="11">
-        <v>43131</v>
-      </c>
-      <c r="I48" s="12"/>
-      <c r="J48" s="13"/>
+        <v>43125</v>
+      </c>
+      <c r="I48" s="11">
+        <v>43125</v>
+      </c>
+      <c r="J48" s="17">
+        <v>1</v>
+      </c>
       <c r="K48" s="19" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
@@ -3909,25 +3969,33 @@
       <c r="AQ48" s="15"/>
       <c r="AR48" s="15"/>
     </row>
-    <row r="49" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
-      <c r="B49" s="9"/>
+      <c r="B49" s="18"/>
       <c r="C49" s="9" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
+      <c r="E49" s="10">
+        <v>14</v>
+      </c>
       <c r="F49" s="11">
-        <v>43126</v>
-      </c>
-      <c r="G49" s="11"/>
+        <v>43080</v>
+      </c>
+      <c r="G49" s="11">
+        <v>43080</v>
+      </c>
       <c r="H49" s="11">
-        <v>43131</v>
-      </c>
-      <c r="I49" s="12"/>
-      <c r="J49" s="13"/>
+        <v>43125</v>
+      </c>
+      <c r="I49" s="11">
+        <v>43125</v>
+      </c>
+      <c r="J49" s="17">
+        <v>1</v>
+      </c>
       <c r="K49" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
@@ -3963,25 +4031,33 @@
       <c r="AQ49" s="15"/>
       <c r="AR49" s="15"/>
     </row>
-    <row r="50" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
-      <c r="B50" s="9"/>
+      <c r="B50" s="18"/>
       <c r="C50" s="9" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
+      <c r="E50" s="10">
+        <v>7</v>
+      </c>
       <c r="F50" s="11">
-        <v>43126</v>
-      </c>
-      <c r="G50" s="11"/>
+        <v>43080</v>
+      </c>
+      <c r="G50" s="11">
+        <v>43080</v>
+      </c>
       <c r="H50" s="11">
-        <v>43131</v>
-      </c>
-      <c r="I50" s="12"/>
-      <c r="J50" s="13"/>
+        <v>43125</v>
+      </c>
+      <c r="I50" s="11">
+        <v>43125</v>
+      </c>
+      <c r="J50" s="17">
+        <v>1</v>
+      </c>
       <c r="K50" s="19" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
@@ -4017,25 +4093,29 @@
       <c r="AQ50" s="15"/>
       <c r="AR50" s="15"/>
     </row>
-    <row r="51" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="B51" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" s="9"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
       <c r="F51" s="11">
         <v>43126</v>
       </c>
-      <c r="G51" s="11"/>
+      <c r="G51" s="11">
+        <v>43126</v>
+      </c>
       <c r="H51" s="11">
         <v>43131</v>
       </c>
-      <c r="I51" s="12"/>
-      <c r="J51" s="13"/>
+      <c r="I51" s="11">
+        <v>43131</v>
+      </c>
+      <c r="J51" s="43"/>
       <c r="K51" s="19" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
@@ -4057,7 +4137,7 @@
       <c r="AC51" s="15"/>
       <c r="AD51" s="15"/>
       <c r="AE51" s="15"/>
-      <c r="AF51" s="15"/>
+      <c r="AF51" s="29"/>
       <c r="AG51" s="15"/>
       <c r="AH51" s="15"/>
       <c r="AI51" s="15"/>
@@ -4075,21 +4155,29 @@
       <c r="A52" s="8"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
+      <c r="E52" s="10">
+        <v>1</v>
+      </c>
       <c r="F52" s="11">
         <v>43126</v>
       </c>
-      <c r="G52" s="11"/>
+      <c r="G52" s="11">
+        <v>43126</v>
+      </c>
       <c r="H52" s="11">
         <v>43131</v>
       </c>
-      <c r="I52" s="12"/>
-      <c r="J52" s="13"/>
+      <c r="I52" s="11">
+        <v>43131</v>
+      </c>
+      <c r="J52" s="17">
+        <v>1</v>
+      </c>
       <c r="K52" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
@@ -4125,25 +4213,33 @@
       <c r="AQ52" s="15"/>
       <c r="AR52" s="15"/>
     </row>
-    <row r="53" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
-      <c r="B53" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
+      <c r="E53" s="10">
+        <v>1</v>
+      </c>
       <c r="F53" s="11">
         <v>43126</v>
       </c>
-      <c r="G53" s="11"/>
+      <c r="G53" s="11">
+        <v>43126</v>
+      </c>
       <c r="H53" s="11">
-        <v>43154</v>
-      </c>
-      <c r="I53" s="12"/>
-      <c r="J53" s="13"/>
+        <v>43131</v>
+      </c>
+      <c r="I53" s="11">
+        <v>43131</v>
+      </c>
+      <c r="J53" s="17">
+        <v>1</v>
+      </c>
       <c r="K53" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
@@ -4179,25 +4275,33 @@
       <c r="AQ53" s="15"/>
       <c r="AR53" s="15"/>
     </row>
-    <row r="54" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
-      <c r="B54" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
+      <c r="E54" s="10">
+        <v>1</v>
+      </c>
       <c r="F54" s="11">
-        <v>43155</v>
-      </c>
-      <c r="G54" s="11"/>
+        <v>43126</v>
+      </c>
+      <c r="G54" s="11">
+        <v>43126</v>
+      </c>
       <c r="H54" s="11">
-        <v>43161</v>
-      </c>
-      <c r="I54" s="12"/>
-      <c r="J54" s="13"/>
+        <v>43131</v>
+      </c>
+      <c r="I54" s="11">
+        <v>43131</v>
+      </c>
+      <c r="J54" s="17">
+        <v>1</v>
+      </c>
       <c r="K54" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -4233,25 +4337,33 @@
       <c r="AQ54" s="15"/>
       <c r="AR54" s="15"/>
     </row>
-    <row r="55" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
-      <c r="B55" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
+      <c r="E55" s="10">
+        <v>1</v>
+      </c>
       <c r="F55" s="11">
-        <v>43173</v>
-      </c>
-      <c r="G55" s="11"/>
+        <v>43126</v>
+      </c>
+      <c r="G55" s="11">
+        <v>43126</v>
+      </c>
       <c r="H55" s="11">
-        <v>43174</v>
-      </c>
-      <c r="I55" s="12"/>
-      <c r="J55" s="13"/>
+        <v>43131</v>
+      </c>
+      <c r="I55" s="11">
+        <v>43131</v>
+      </c>
+      <c r="J55" s="17">
+        <v>1</v>
+      </c>
       <c r="K55" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
@@ -4287,24 +4399,34 @@
       <c r="AQ55" s="15"/>
       <c r="AR55" s="15"/>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A56" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="B56" s="9"/>
+    <row r="56" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="C56" s="9"/>
       <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
+      <c r="E56" s="10">
+        <v>15</v>
+      </c>
       <c r="F56" s="11">
-        <v>43190</v>
-      </c>
-      <c r="G56" s="11"/>
+        <v>43131</v>
+      </c>
+      <c r="G56" s="11">
+        <v>43131</v>
+      </c>
       <c r="H56" s="11">
-        <v>43194</v>
-      </c>
-      <c r="I56" s="12"/>
-      <c r="J56" s="13"/>
-      <c r="K56" s="19"/>
+        <v>43154</v>
+      </c>
+      <c r="I56" s="11">
+        <v>43184</v>
+      </c>
+      <c r="J56" s="42">
+        <v>1</v>
+      </c>
+      <c r="K56" s="19" t="s">
+        <v>35</v>
+      </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
       <c r="N56" s="15"/>
@@ -4325,39 +4447,47 @@
       <c r="AC56" s="15"/>
       <c r="AD56" s="15"/>
       <c r="AE56" s="15"/>
-      <c r="AF56" s="15"/>
-      <c r="AG56" s="15"/>
-      <c r="AH56" s="15"/>
-      <c r="AI56" s="15"/>
+      <c r="AF56" s="29"/>
+      <c r="AG56" s="29"/>
+      <c r="AH56" s="29"/>
+      <c r="AI56" s="29"/>
       <c r="AJ56" s="15"/>
       <c r="AK56" s="15"/>
       <c r="AL56" s="15"/>
       <c r="AM56" s="15"/>
-      <c r="AN56" s="29"/>
-      <c r="AO56" s="29"/>
+      <c r="AN56" s="15"/>
+      <c r="AO56" s="15"/>
       <c r="AP56" s="15"/>
       <c r="AQ56" s="15"/>
       <c r="AR56" s="15"/>
     </row>
     <row r="57" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
-      <c r="B57" s="9" t="s">
-        <v>19</v>
+      <c r="B57" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
+      <c r="E57" s="10">
+        <v>4</v>
+      </c>
       <c r="F57" s="11">
-        <v>43190</v>
-      </c>
-      <c r="G57" s="11"/>
+        <v>43155</v>
+      </c>
+      <c r="G57" s="11">
+        <v>43185</v>
+      </c>
       <c r="H57" s="11">
-        <v>43192</v>
-      </c>
-      <c r="I57" s="12"/>
-      <c r="J57" s="13"/>
+        <v>43161</v>
+      </c>
+      <c r="I57" s="12">
+        <v>43186</v>
+      </c>
+      <c r="J57" s="42">
+        <v>1</v>
+      </c>
       <c r="K57" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
@@ -4383,8 +4513,8 @@
       <c r="AG57" s="15"/>
       <c r="AH57" s="15"/>
       <c r="AI57" s="15"/>
-      <c r="AJ57" s="15"/>
-      <c r="AK57" s="15"/>
+      <c r="AJ57" s="29"/>
+      <c r="AK57" s="29"/>
       <c r="AL57" s="15"/>
       <c r="AM57" s="15"/>
       <c r="AN57" s="15"/>
@@ -4395,23 +4525,31 @@
     </row>
     <row r="58" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
-      <c r="B58" s="9" t="s">
-        <v>20</v>
+      <c r="B58" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
+      <c r="E58" s="10">
+        <v>1</v>
+      </c>
       <c r="F58" s="11">
-        <v>43190</v>
-      </c>
-      <c r="G58" s="11"/>
+        <v>43173</v>
+      </c>
+      <c r="G58" s="11">
+        <v>43187</v>
+      </c>
       <c r="H58" s="11">
+        <v>43174</v>
+      </c>
+      <c r="I58" s="12">
         <v>43194</v>
       </c>
-      <c r="I58" s="12"/>
-      <c r="J58" s="13"/>
+      <c r="J58" s="42">
+        <v>1</v>
+      </c>
       <c r="K58" s="19" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -4439,7 +4577,7 @@
       <c r="AI58" s="15"/>
       <c r="AJ58" s="15"/>
       <c r="AK58" s="15"/>
-      <c r="AL58" s="15"/>
+      <c r="AL58" s="29"/>
       <c r="AM58" s="15"/>
       <c r="AN58" s="15"/>
       <c r="AO58" s="15"/>
@@ -4447,26 +4585,28 @@
       <c r="AQ58" s="15"/>
       <c r="AR58" s="15"/>
     </row>
-    <row r="59" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="8"/>
-      <c r="B59" s="9" t="s">
-        <v>24</v>
-      </c>
+    <row r="59" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A59" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="9"/>
       <c r="C59" s="9"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
       <c r="F59" s="11">
         <v>43190</v>
       </c>
-      <c r="G59" s="11"/>
+      <c r="G59" s="11">
+        <v>43192</v>
+      </c>
       <c r="H59" s="11">
         <v>43194</v>
       </c>
-      <c r="I59" s="12"/>
-      <c r="J59" s="13"/>
-      <c r="K59" s="19" t="s">
-        <v>70</v>
-      </c>
+      <c r="I59" s="12">
+        <v>43202</v>
+      </c>
+      <c r="J59" s="44"/>
+      <c r="K59" s="19"/>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
@@ -4495,31 +4635,39 @@
       <c r="AK59" s="15"/>
       <c r="AL59" s="15"/>
       <c r="AM59" s="15"/>
-      <c r="AN59" s="15"/>
-      <c r="AO59" s="15"/>
+      <c r="AN59" s="29"/>
+      <c r="AO59" s="29"/>
       <c r="AP59" s="15"/>
       <c r="AQ59" s="15"/>
       <c r="AR59" s="15"/>
     </row>
-    <row r="60" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="B60" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C60" s="9"/>
       <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
+      <c r="E60" s="10">
+        <v>2</v>
+      </c>
       <c r="F60" s="11">
         <v>43190</v>
       </c>
-      <c r="G60" s="11"/>
+      <c r="G60" s="11">
+        <v>43192</v>
+      </c>
       <c r="H60" s="11">
-        <v>43194</v>
-      </c>
-      <c r="I60" s="12"/>
-      <c r="J60" s="13"/>
+        <v>43192</v>
+      </c>
+      <c r="I60" s="12">
+        <v>43202</v>
+      </c>
+      <c r="J60" s="42">
+        <v>1</v>
+      </c>
       <c r="K60" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
@@ -4555,25 +4703,33 @@
       <c r="AQ60" s="15"/>
       <c r="AR60" s="15"/>
     </row>
-    <row r="61" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="B61" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="9"/>
       <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
+      <c r="E61" s="10">
+        <v>2</v>
+      </c>
       <c r="F61" s="11">
         <v>43190</v>
       </c>
-      <c r="G61" s="11"/>
+      <c r="G61" s="11">
+        <v>43192</v>
+      </c>
       <c r="H61" s="11">
         <v>43194</v>
       </c>
-      <c r="I61" s="12"/>
-      <c r="J61" s="13"/>
+      <c r="I61" s="12">
+        <v>43202</v>
+      </c>
+      <c r="J61" s="42">
+        <v>1</v>
+      </c>
       <c r="K61" s="19" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
@@ -4609,24 +4765,30 @@
       <c r="AQ61" s="15"/>
       <c r="AR61" s="15"/>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B62" s="9"/>
+    <row r="62" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8"/>
+      <c r="B62" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
       <c r="F62" s="11">
-        <v>43073</v>
-      </c>
-      <c r="G62" s="11"/>
+        <v>43190</v>
+      </c>
+      <c r="G62" s="11">
+        <v>43211</v>
+      </c>
       <c r="H62" s="11">
-        <v>43217</v>
-      </c>
-      <c r="I62" s="12"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="19"/>
+        <v>43194</v>
+      </c>
+      <c r="I62" s="11">
+        <v>43211</v>
+      </c>
+      <c r="J62" s="44"/>
+      <c r="K62" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
@@ -4642,44 +4804,52 @@
       <c r="X62" s="15"/>
       <c r="Y62" s="15"/>
       <c r="Z62" s="15"/>
-      <c r="AA62" s="29"/>
-      <c r="AB62" s="29"/>
-      <c r="AC62" s="29"/>
-      <c r="AD62" s="29"/>
-      <c r="AE62" s="29"/>
-      <c r="AF62" s="29"/>
-      <c r="AG62" s="29"/>
-      <c r="AH62" s="29"/>
-      <c r="AI62" s="29"/>
-      <c r="AJ62" s="29"/>
-      <c r="AK62" s="29"/>
-      <c r="AL62" s="29"/>
-      <c r="AM62" s="29"/>
-      <c r="AN62" s="29"/>
-      <c r="AO62" s="29"/>
-      <c r="AP62" s="29"/>
-      <c r="AQ62" s="29"/>
-      <c r="AR62" s="29"/>
-    </row>
-    <row r="63" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="AA62" s="15"/>
+      <c r="AB62" s="15"/>
+      <c r="AC62" s="15"/>
+      <c r="AD62" s="15"/>
+      <c r="AE62" s="15"/>
+      <c r="AF62" s="15"/>
+      <c r="AG62" s="15"/>
+      <c r="AH62" s="15"/>
+      <c r="AI62" s="15"/>
+      <c r="AJ62" s="15"/>
+      <c r="AK62" s="15"/>
+      <c r="AL62" s="15"/>
+      <c r="AM62" s="15"/>
+      <c r="AN62" s="15"/>
+      <c r="AO62" s="15"/>
+      <c r="AP62" s="15"/>
+      <c r="AQ62" s="15"/>
+      <c r="AR62" s="15"/>
+    </row>
+    <row r="63" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="9"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="D63" s="10"/>
-      <c r="E63" s="10"/>
+      <c r="E63" s="10">
+        <v>1</v>
+      </c>
       <c r="F63" s="11">
-        <v>43161</v>
-      </c>
-      <c r="G63" s="11"/>
+        <v>43190</v>
+      </c>
+      <c r="G63" s="11">
+        <v>43211</v>
+      </c>
       <c r="H63" s="11">
-        <v>43189</v>
-      </c>
-      <c r="I63" s="12"/>
-      <c r="J63" s="13"/>
+        <v>43194</v>
+      </c>
+      <c r="I63" s="11">
+        <v>43211</v>
+      </c>
+      <c r="J63" s="42">
+        <v>1</v>
+      </c>
       <c r="K63" s="19" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
@@ -4715,23 +4885,31 @@
       <c r="AQ63" s="15"/>
       <c r="AR63" s="15"/>
     </row>
-    <row r="64" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9" t="s">
+        <v>26</v>
+      </c>
       <c r="D64" s="10"/>
-      <c r="E64" s="10"/>
+      <c r="E64" s="10">
+        <v>1</v>
+      </c>
       <c r="F64" s="11">
-        <v>43073</v>
-      </c>
-      <c r="G64" s="11"/>
+        <v>43190</v>
+      </c>
+      <c r="G64" s="11">
+        <v>43211</v>
+      </c>
       <c r="H64" s="11">
-        <v>43217</v>
-      </c>
-      <c r="I64" s="12"/>
-      <c r="J64" s="13"/>
+        <v>43194</v>
+      </c>
+      <c r="I64" s="11">
+        <v>43211</v>
+      </c>
+      <c r="J64" s="42">
+        <v>1</v>
+      </c>
       <c r="K64" s="19" t="s">
         <v>35</v>
       </c>
@@ -4769,16 +4947,14 @@
       <c r="AQ64" s="15"/>
       <c r="AR64" s="15"/>
     </row>
-    <row r="65" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
+    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A65" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="B65" s="9"/>
-      <c r="C65" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="C65" s="9"/>
       <c r="D65" s="10"/>
-      <c r="E65" s="10">
-        <v>2</v>
-      </c>
+      <c r="E65" s="10"/>
       <c r="F65" s="11">
         <v>43073</v>
       </c>
@@ -4786,17 +4962,11 @@
         <v>43073</v>
       </c>
       <c r="H65" s="11">
-        <v>43077</v>
-      </c>
-      <c r="I65" s="11">
-        <v>43077</v>
-      </c>
-      <c r="J65" s="17">
-        <v>1</v>
-      </c>
-      <c r="K65" s="19" t="s">
-        <v>36</v>
-      </c>
+        <v>43217</v>
+      </c>
+      <c r="I65" s="12"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="19"/>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
@@ -4812,44 +4982,52 @@
       <c r="X65" s="15"/>
       <c r="Y65" s="15"/>
       <c r="Z65" s="15"/>
-      <c r="AA65" s="15"/>
-      <c r="AB65" s="15"/>
-      <c r="AC65" s="15"/>
-      <c r="AD65" s="15"/>
-      <c r="AE65" s="15"/>
-      <c r="AF65" s="15"/>
-      <c r="AG65" s="15"/>
-      <c r="AH65" s="15"/>
-      <c r="AI65" s="15"/>
-      <c r="AJ65" s="15"/>
-      <c r="AK65" s="15"/>
-      <c r="AL65" s="15"/>
-      <c r="AM65" s="15"/>
-      <c r="AN65" s="15"/>
-      <c r="AO65" s="15"/>
-      <c r="AP65" s="15"/>
-      <c r="AQ65" s="15"/>
-      <c r="AR65" s="15"/>
-    </row>
-    <row r="66" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="AA65" s="29"/>
+      <c r="AB65" s="29"/>
+      <c r="AC65" s="29"/>
+      <c r="AD65" s="29"/>
+      <c r="AE65" s="29"/>
+      <c r="AF65" s="29"/>
+      <c r="AG65" s="29"/>
+      <c r="AH65" s="29"/>
+      <c r="AI65" s="29"/>
+      <c r="AJ65" s="29"/>
+      <c r="AK65" s="29"/>
+      <c r="AL65" s="29"/>
+      <c r="AM65" s="29"/>
+      <c r="AN65" s="29"/>
+      <c r="AO65" s="29"/>
+      <c r="AP65" s="29"/>
+      <c r="AQ65" s="29"/>
+      <c r="AR65" s="29"/>
+    </row>
+    <row r="66" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="B66" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C66" s="9"/>
       <c r="D66" s="10"/>
-      <c r="E66" s="10"/>
+      <c r="E66" s="10">
+        <v>10</v>
+      </c>
       <c r="F66" s="11">
-        <v>43206</v>
-      </c>
-      <c r="G66" s="11"/>
+        <v>43161</v>
+      </c>
+      <c r="G66" s="11">
+        <v>43161</v>
+      </c>
       <c r="H66" s="11">
-        <v>43217</v>
-      </c>
-      <c r="I66" s="12"/>
-      <c r="J66" s="13"/>
+        <v>43203</v>
+      </c>
+      <c r="I66" s="12">
+        <v>43203</v>
+      </c>
+      <c r="J66" s="17">
+        <v>1</v>
+      </c>
       <c r="K66" s="19" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
@@ -4885,25 +5063,27 @@
       <c r="AQ66" s="15"/>
       <c r="AR66" s="15"/>
     </row>
-    <row r="67" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="18" t="s">
-        <v>63</v>
-      </c>
+      <c r="B67" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C67" s="9"/>
       <c r="D67" s="10"/>
       <c r="E67" s="10"/>
       <c r="F67" s="11">
-        <v>43206</v>
-      </c>
-      <c r="G67" s="11"/>
+        <v>43073</v>
+      </c>
+      <c r="G67" s="11">
+        <v>43073</v>
+      </c>
       <c r="H67" s="11">
         <v>43217</v>
       </c>
       <c r="I67" s="12"/>
       <c r="J67" s="13"/>
       <c r="K67" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L67" s="15"/>
       <c r="M67" s="15"/>
@@ -4939,33 +5119,33 @@
       <c r="AQ67" s="15"/>
       <c r="AR67" s="15"/>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>84</v>
-      </c>
+    <row r="68" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
       <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
+      <c r="C68" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="D68" s="10"/>
       <c r="E68" s="10">
         <v>2</v>
       </c>
       <c r="F68" s="11">
-        <v>43038</v>
+        <v>43073</v>
       </c>
       <c r="G68" s="11">
-        <v>43038</v>
+        <v>43073</v>
       </c>
       <c r="H68" s="11">
-        <v>43039</v>
+        <v>43077</v>
       </c>
       <c r="I68" s="11">
-        <v>43039</v>
+        <v>43077</v>
       </c>
       <c r="J68" s="17">
         <v>1</v>
       </c>
-      <c r="K68" s="14" t="s">
-        <v>34</v>
+      <c r="K68" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
@@ -4977,7 +5157,7 @@
       <c r="S68" s="15"/>
       <c r="T68" s="15"/>
       <c r="U68" s="15"/>
-      <c r="V68" s="29"/>
+      <c r="V68" s="15"/>
       <c r="W68" s="15"/>
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
@@ -5001,33 +5181,29 @@
       <c r="AQ68" s="15"/>
       <c r="AR68" s="15"/>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A69" s="8" t="s">
-        <v>85</v>
-      </c>
+    <row r="69" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
       <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
+      <c r="C69" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="D69" s="10"/>
       <c r="E69" s="10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F69" s="11">
-        <v>43048</v>
+        <v>43206</v>
       </c>
       <c r="G69" s="11">
-        <v>43048</v>
+        <v>43206</v>
       </c>
       <c r="H69" s="11">
-        <v>43051</v>
-      </c>
-      <c r="I69" s="11">
-        <v>43051</v>
-      </c>
-      <c r="J69" s="17">
-        <v>1</v>
-      </c>
-      <c r="K69" s="14" t="s">
-        <v>34</v>
+        <v>43217</v>
+      </c>
+      <c r="I69" s="12"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="19" t="s">
+        <v>35</v>
       </c>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
@@ -5041,8 +5217,8 @@
       <c r="U69" s="15"/>
       <c r="V69" s="15"/>
       <c r="W69" s="15"/>
-      <c r="X69" s="29"/>
-      <c r="Y69" s="29"/>
+      <c r="X69" s="15"/>
+      <c r="Y69" s="15"/>
       <c r="Z69" s="15"/>
       <c r="AA69" s="15"/>
       <c r="AB69" s="15"/>
@@ -5063,6 +5239,315 @@
       <c r="AQ69" s="15"/>
       <c r="AR69" s="15"/>
     </row>
+    <row r="70" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10">
+        <v>3</v>
+      </c>
+      <c r="F70" s="11">
+        <v>43206</v>
+      </c>
+      <c r="G70" s="11">
+        <v>43206</v>
+      </c>
+      <c r="H70" s="11">
+        <v>43217</v>
+      </c>
+      <c r="I70" s="12"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+      <c r="S70" s="15"/>
+      <c r="T70" s="15"/>
+      <c r="U70" s="15"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="15"/>
+      <c r="X70" s="15"/>
+      <c r="Y70" s="15"/>
+      <c r="Z70" s="15"/>
+      <c r="AA70" s="15"/>
+      <c r="AB70" s="15"/>
+      <c r="AC70" s="15"/>
+      <c r="AD70" s="15"/>
+      <c r="AE70" s="15"/>
+      <c r="AF70" s="15"/>
+      <c r="AG70" s="15"/>
+      <c r="AH70" s="15"/>
+      <c r="AI70" s="15"/>
+      <c r="AJ70" s="15"/>
+      <c r="AK70" s="15"/>
+      <c r="AL70" s="15"/>
+      <c r="AM70" s="15"/>
+      <c r="AN70" s="15"/>
+      <c r="AO70" s="15"/>
+      <c r="AP70" s="15"/>
+      <c r="AQ70" s="15"/>
+      <c r="AR70" s="15"/>
+    </row>
+    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A71" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" s="9"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10">
+        <v>2</v>
+      </c>
+      <c r="F71" s="11">
+        <v>43199</v>
+      </c>
+      <c r="G71" s="11">
+        <v>43199</v>
+      </c>
+      <c r="H71" s="11">
+        <v>43203</v>
+      </c>
+      <c r="I71" s="11">
+        <v>43202</v>
+      </c>
+      <c r="J71" s="17">
+        <v>1</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+      <c r="U71" s="15"/>
+      <c r="V71" s="29"/>
+      <c r="W71" s="15"/>
+      <c r="X71" s="15"/>
+      <c r="Y71" s="15"/>
+      <c r="Z71" s="15"/>
+      <c r="AA71" s="15"/>
+      <c r="AB71" s="15"/>
+      <c r="AC71" s="15"/>
+      <c r="AD71" s="15"/>
+      <c r="AE71" s="15"/>
+      <c r="AF71" s="15"/>
+      <c r="AG71" s="15"/>
+      <c r="AH71" s="15"/>
+      <c r="AI71" s="15"/>
+      <c r="AJ71" s="15"/>
+      <c r="AK71" s="15"/>
+      <c r="AL71" s="15"/>
+      <c r="AM71" s="15"/>
+      <c r="AN71" s="15"/>
+      <c r="AO71" s="15"/>
+      <c r="AP71" s="15"/>
+      <c r="AQ71" s="15"/>
+      <c r="AR71" s="15"/>
+    </row>
+    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A72" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" s="9"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="11">
+        <v>43048</v>
+      </c>
+      <c r="G72" s="11">
+        <v>43048</v>
+      </c>
+      <c r="H72" s="11">
+        <v>43190</v>
+      </c>
+      <c r="I72" s="11">
+        <v>43190</v>
+      </c>
+      <c r="J72" s="43"/>
+      <c r="K72" s="14"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="15"/>
+      <c r="X72" s="28"/>
+      <c r="Y72" s="28"/>
+      <c r="Z72" s="15"/>
+      <c r="AA72" s="15"/>
+      <c r="AB72" s="15"/>
+      <c r="AC72" s="15"/>
+      <c r="AD72" s="15"/>
+      <c r="AE72" s="15"/>
+      <c r="AF72" s="15"/>
+      <c r="AG72" s="15"/>
+      <c r="AH72" s="15"/>
+      <c r="AI72" s="15"/>
+      <c r="AJ72" s="15"/>
+      <c r="AK72" s="15"/>
+      <c r="AL72" s="15"/>
+      <c r="AM72" s="15"/>
+      <c r="AN72" s="15"/>
+      <c r="AO72" s="15"/>
+      <c r="AP72" s="15"/>
+      <c r="AQ72" s="15"/>
+      <c r="AR72" s="15"/>
+    </row>
+    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A73" s="8"/>
+      <c r="B73" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10">
+        <v>5</v>
+      </c>
+      <c r="F73" s="11">
+        <v>43048</v>
+      </c>
+      <c r="G73" s="11">
+        <v>43048</v>
+      </c>
+      <c r="H73" s="11">
+        <v>43051</v>
+      </c>
+      <c r="I73" s="11">
+        <v>43051</v>
+      </c>
+      <c r="J73" s="17">
+        <v>1</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="28"/>
+      <c r="Y73" s="29"/>
+      <c r="Z73" s="15"/>
+      <c r="AA73" s="15"/>
+      <c r="AB73" s="15"/>
+      <c r="AC73" s="15"/>
+      <c r="AD73" s="15"/>
+      <c r="AE73" s="15"/>
+      <c r="AF73" s="15"/>
+      <c r="AG73" s="15"/>
+      <c r="AH73" s="15"/>
+      <c r="AI73" s="15"/>
+      <c r="AJ73" s="15"/>
+      <c r="AK73" s="15"/>
+      <c r="AL73" s="15"/>
+      <c r="AM73" s="15"/>
+      <c r="AN73" s="15"/>
+      <c r="AO73" s="15"/>
+      <c r="AP73" s="15"/>
+      <c r="AQ73" s="15"/>
+      <c r="AR73" s="15"/>
+    </row>
+    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="B74" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C74" s="9"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10">
+        <v>4</v>
+      </c>
+      <c r="F74" s="11">
+        <v>43185</v>
+      </c>
+      <c r="G74" s="11">
+        <v>43185</v>
+      </c>
+      <c r="H74" s="11">
+        <v>43190</v>
+      </c>
+      <c r="I74" s="11">
+        <v>43190</v>
+      </c>
+      <c r="J74" s="17">
+        <v>1</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+      <c r="U74" s="15"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="15"/>
+      <c r="X74" s="28"/>
+      <c r="Y74" s="28"/>
+      <c r="Z74" s="15"/>
+      <c r="AA74" s="15"/>
+      <c r="AB74" s="15"/>
+      <c r="AC74" s="15"/>
+      <c r="AD74" s="15"/>
+      <c r="AE74" s="15"/>
+      <c r="AF74" s="15"/>
+      <c r="AG74" s="15"/>
+      <c r="AH74" s="15"/>
+      <c r="AI74" s="15"/>
+      <c r="AJ74" s="15"/>
+      <c r="AK74" s="15"/>
+      <c r="AL74" s="15"/>
+      <c r="AM74" s="15"/>
+      <c r="AN74" s="29"/>
+      <c r="AO74" s="15"/>
+      <c r="AP74" s="15"/>
+      <c r="AQ74" s="15"/>
+      <c r="AR74" s="15"/>
+    </row>
+    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="D75" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E75" s="45">
+        <f>SUM(E3:E74)</f>
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:D2"/>

</xml_diff>

<commit_message>
Updated WBS Project Plan
added Section 4.0 on WP/PHP, WAMP Training
</commit_message>
<xml_diff>
--- a/2017-18 SGW WBS Project Plan.xlsx
+++ b/2017-18 SGW WBS Project Plan.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenelazo\Documents\GitHub\MIST7590-Smithgall-Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66342C6A-CA07-43D8-A6BB-BD12AA61CE56}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="60" windowWidth="20736" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="60" windowWidth="20730" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="102">
   <si>
     <t>Planned Start Date</t>
   </si>
@@ -70,48 +64,6 @@
     <t xml:space="preserve">Completion Percentage </t>
   </si>
   <si>
-    <t>4.1  Create the Database</t>
-  </si>
-  <si>
-    <t>4.1.1  Load constant/attribute values</t>
-  </si>
-  <si>
-    <t>4.3.1  Test Application Flow</t>
-  </si>
-  <si>
-    <t>4.3.2  Test Application Content</t>
-  </si>
-  <si>
-    <t>4.3.4  Adjust Application</t>
-  </si>
-  <si>
-    <t>4.3.3  Test Application Logic</t>
-  </si>
-  <si>
-    <t>5.1  Prep Code for Move to Production</t>
-  </si>
-  <si>
-    <t>5.2  Move to Production</t>
-  </si>
-  <si>
-    <t>6.0  Develop Project Communication Material</t>
-  </si>
-  <si>
-    <t>6.2.1  Develop Term I Project Binder</t>
-  </si>
-  <si>
-    <t>6.2.2  Develop Term II Project Binder</t>
-  </si>
-  <si>
-    <t>5.3  Transfer Ownership to Client</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.3.1  Train Client </t>
-  </si>
-  <si>
-    <t>5.3.2  Transfer electronic content to client</t>
-  </si>
-  <si>
     <t>2.1.1  Develop Work Breakdown Structure</t>
   </si>
   <si>
@@ -214,42 +166,18 @@
     <t>Eliseo, Clark</t>
   </si>
   <si>
-    <t>6.2.3  Develop Final Project Presentation</t>
-  </si>
-  <si>
     <t>2.4 Research Web CMS tool and Site Host</t>
   </si>
   <si>
-    <t>4.4 Write the Code - Increment 2</t>
-  </si>
-  <si>
-    <t>4.5 Test the Site and App - Increment 2</t>
-  </si>
-  <si>
-    <t>4.3 Test the Site and App - Increment 1</t>
-  </si>
-  <si>
-    <t>4.2  Write the Code - Increment 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.6  Conduct Stakeholder Review </t>
-  </si>
-  <si>
     <t>Eliseo, Jennifer</t>
   </si>
   <si>
     <t>Andrea, Clark</t>
   </si>
   <si>
-    <t>6.2  Develop Project Deliverables</t>
-  </si>
-  <si>
     <t>3.1.1  Build basic website for text/photo update</t>
   </si>
   <si>
-    <t>5.0  Deploy Website and Volunteer Application</t>
-  </si>
-  <si>
     <t>3.2  Develop test cases for Wordpress site update</t>
   </si>
   <si>
@@ -277,27 +205,9 @@
     <t>1.2.7.2  Obtain Stakeholder Approval</t>
   </si>
   <si>
-    <t>7.0 Update PHP, WordPress Themes &amp; Plugins (Site Maintenance)</t>
-  </si>
-  <si>
-    <t>8.0 Restore Volunteer Reports site (Site Maintenance)</t>
-  </si>
-  <si>
     <t>1.2.2 Define Security Remediation Plan (Site Maintenance)</t>
   </si>
   <si>
-    <t>4.0  Build and Test the Site &amp; Volunteer Application</t>
-  </si>
-  <si>
-    <t>6.1  Develop User Guides and Video Tutorials</t>
-  </si>
-  <si>
-    <t>8.1  Rebuild Reports site using PHPRunner (free version)</t>
-  </si>
-  <si>
-    <t>8.2  Update site to add Section field (SGW &amp; Hardman Farm)</t>
-  </si>
-  <si>
     <t>Eliseo, Andrea</t>
   </si>
   <si>
@@ -313,25 +223,118 @@
     <t>3.4  Conduct test and record test results</t>
   </si>
   <si>
-    <t>4.2.1  Use current WordPress to rebuild site</t>
-  </si>
-  <si>
-    <t>4.2.2  Use plugins to build Volunteer app in WP</t>
-  </si>
-  <si>
-    <t>4.2.3  Rebuild app as standalone with MySQLi</t>
-  </si>
-  <si>
     <t>Jennifer, Eliseo</t>
   </si>
   <si>
     <t>TOTAL DURATION (hr)</t>
+  </si>
+  <si>
+    <t>4.0  Complete Training through Lynda.com</t>
+  </si>
+  <si>
+    <t>4.1  Go through training tutorials on WordPress and PHP</t>
+  </si>
+  <si>
+    <t>4.2  Complete training tutorials on WAMP Server</t>
+  </si>
+  <si>
+    <t>5.0  Build and Test the Site &amp; Volunteer Application</t>
+  </si>
+  <si>
+    <t>5.1  Create the Database</t>
+  </si>
+  <si>
+    <t>5.2  Write the Code - Increment 1</t>
+  </si>
+  <si>
+    <t>5.1.1  Load constant/attribute values</t>
+  </si>
+  <si>
+    <t>5.2.1  Use current WordPress to rebuild site</t>
+  </si>
+  <si>
+    <t>5.2.2  Use plugins to build Volunteer app in WP</t>
+  </si>
+  <si>
+    <t>5.2.3  Rebuild app as standalone with MySQLi</t>
+  </si>
+  <si>
+    <t>5.3 Test the Site and App - Increment 1</t>
+  </si>
+  <si>
+    <t>5.3.1  Test Application Flow</t>
+  </si>
+  <si>
+    <t>5.3.2  Test Application Content</t>
+  </si>
+  <si>
+    <t>5.3.3  Test Application Logic</t>
+  </si>
+  <si>
+    <t>5.3.4  Adjust Application</t>
+  </si>
+  <si>
+    <t>5.4 Write the Code - Increment 2</t>
+  </si>
+  <si>
+    <t>5.5 Test the Site and App - Increment 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.6  Conduct Stakeholder Review </t>
+  </si>
+  <si>
+    <t>6.0  Deploy Website and Volunteer Application</t>
+  </si>
+  <si>
+    <t>6.2  Move to Production</t>
+  </si>
+  <si>
+    <t>6.3  Transfer Ownership to Client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.3.1  Train Client </t>
+  </si>
+  <si>
+    <t>6.3.2  Transfer electronic content to client</t>
+  </si>
+  <si>
+    <t>7.0  Develop Project Communication Material</t>
+  </si>
+  <si>
+    <t>7.1  Develop User Guides and Video Tutorials</t>
+  </si>
+  <si>
+    <t>7.2  Develop Project Deliverables</t>
+  </si>
+  <si>
+    <t>7.2.1  Develop Term I Project Binder</t>
+  </si>
+  <si>
+    <t>7.2.2  Develop Term II Project Binder</t>
+  </si>
+  <si>
+    <t>7.2.3  Develop Final Project Presentation</t>
+  </si>
+  <si>
+    <t>9.0 Restore Volunteer Reports site (Site Maintenance)</t>
+  </si>
+  <si>
+    <t>9.1  Rebuild Reports site using PHPRunner (free version)</t>
+  </si>
+  <si>
+    <t>9.2  Update site to add Section field (SGW &amp; Hardman Farm)</t>
+  </si>
+  <si>
+    <t>8.0 Update PHP, WordPress, Themes &amp; Plugins (Site Maintenance)</t>
+  </si>
+  <si>
+    <t>6.1  Prep Code for Move to Production (Host Server)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
@@ -687,7 +690,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -958,58 +961,58 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BF75"/>
+  <dimension ref="A1:BF78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="11" ySplit="2" topLeftCell="AD54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="2" topLeftCell="L3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F75" sqref="F75"/>
+      <selection pane="bottomRight" activeCell="N80" sqref="N80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" outlineLevelRow="3" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" outlineLevelRow="3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="47.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
-    <col min="8" max="9" width="12.109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" style="2" customWidth="1"/>
-    <col min="13" max="14" width="5.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
+    <col min="8" max="9" width="12.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="5.28515625" style="2" customWidth="1"/>
     <col min="15" max="15" width="5" style="2" customWidth="1"/>
-    <col min="16" max="16" width="5.109375" style="2" customWidth="1"/>
-    <col min="17" max="17" width="5.5546875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="5.44140625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="5.33203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="6.33203125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="6.5546875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="6.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="5.5703125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="5.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="6.28515625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.5703125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" style="2" customWidth="1"/>
     <col min="23" max="24" width="6" style="2" customWidth="1"/>
-    <col min="25" max="27" width="6.33203125" style="2" customWidth="1"/>
-    <col min="28" max="44" width="5.6640625" style="2" customWidth="1"/>
-    <col min="45" max="16384" width="8.88671875" style="2"/>
+    <col min="25" max="27" width="6.28515625" style="2" customWidth="1"/>
+    <col min="28" max="44" width="5.7109375" style="2" customWidth="1"/>
+    <col min="45" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:58" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="40" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -1059,7 +1062,7 @@
       <c r="AQ1" s="45"/>
       <c r="AR1" s="46"/>
     </row>
-    <row r="2" spans="1:58" s="7" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" s="7" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>10</v>
       </c>
@@ -1067,7 +1070,7 @@
       <c r="C2" s="38"/>
       <c r="D2" s="39"/>
       <c r="E2" s="21" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -1201,9 +1204,9 @@
       <c r="BE2" s="6"/>
       <c r="BF2" s="6"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
@@ -1255,10 +1258,10 @@
       <c r="AQ3" s="28"/>
       <c r="AR3" s="28"/>
     </row>
-    <row r="4" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="10"/>
@@ -1281,7 +1284,7 @@
         <v>1</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L4" s="15"/>
       <c r="M4" s="15"/>
@@ -1317,10 +1320,10 @@
       <c r="AQ4" s="15"/>
       <c r="AR4" s="15"/>
     </row>
-    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
@@ -1371,11 +1374,11 @@
       <c r="AQ5" s="15"/>
       <c r="AR5" s="15"/>
     </row>
-    <row r="6" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10">
@@ -1397,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
@@ -1433,11 +1436,11 @@
       <c r="AQ6" s="15"/>
       <c r="AR6" s="15"/>
     </row>
-    <row r="7" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="9"/>
       <c r="C7" s="18" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10">
@@ -1459,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="L7" s="15"/>
       <c r="M7" s="15"/>
@@ -1495,11 +1498,11 @@
       <c r="AQ7" s="15"/>
       <c r="AR7" s="15"/>
     </row>
-    <row r="8" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="9"/>
       <c r="C8" s="18" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10">
@@ -1521,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
@@ -1557,11 +1560,11 @@
       <c r="AQ8" s="15"/>
       <c r="AR8" s="15"/>
     </row>
-    <row r="9" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="9"/>
       <c r="C9" s="18" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10">
@@ -1583,7 +1586,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
@@ -1619,11 +1622,11 @@
       <c r="AQ9" s="15"/>
       <c r="AR9" s="15"/>
     </row>
-    <row r="10" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9"/>
       <c r="C10" s="18" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10">
@@ -1645,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
@@ -1681,11 +1684,11 @@
       <c r="AQ10" s="15"/>
       <c r="AR10" s="15"/>
     </row>
-    <row r="11" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9"/>
       <c r="C11" s="18" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10">
@@ -1707,7 +1710,7 @@
         <v>1</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
@@ -1743,11 +1746,11 @@
       <c r="AQ11" s="15"/>
       <c r="AR11" s="15"/>
     </row>
-    <row r="12" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:58" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9"/>
       <c r="C12" s="18" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
@@ -1763,7 +1766,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="31"/>
       <c r="K12" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
@@ -1799,12 +1802,12 @@
       <c r="AQ12" s="15"/>
       <c r="AR12" s="15"/>
     </row>
-    <row r="13" spans="1:58" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:58" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="27" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E13" s="10">
         <v>2</v>
@@ -1825,7 +1828,7 @@
         <v>1</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
@@ -1861,12 +1864,12 @@
       <c r="AQ13" s="15"/>
       <c r="AR13" s="15"/>
     </row>
-    <row r="14" spans="1:58" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:58" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="27" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="E14" s="10">
         <v>2</v>
@@ -1882,10 +1885,10 @@
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="25" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
@@ -1921,7 +1924,7 @@
       <c r="AQ14" s="15"/>
       <c r="AR14" s="15"/>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
@@ -1977,7 +1980,7 @@
       <c r="AQ15" s="15"/>
       <c r="AR15" s="15"/>
     </row>
-    <row r="16" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:58" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="9" t="s">
         <v>6</v>
@@ -2033,11 +2036,11 @@
       <c r="AQ16" s="15"/>
       <c r="AR16" s="15"/>
     </row>
-    <row r="17" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10">
@@ -2059,7 +2062,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
@@ -2095,7 +2098,7 @@
       <c r="AQ17" s="15"/>
       <c r="AR17" s="15"/>
     </row>
-    <row r="18" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9" t="s">
@@ -2121,7 +2124,7 @@
         <v>1</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
@@ -2157,11 +2160,11 @@
       <c r="AQ18" s="15"/>
       <c r="AR18" s="15"/>
     </row>
-    <row r="19" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10">
@@ -2183,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
@@ -2219,7 +2222,7 @@
       <c r="AQ19" s="15"/>
       <c r="AR19" s="15"/>
     </row>
-    <row r="20" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="9" t="s">
         <v>8</v>
@@ -2275,7 +2278,7 @@
       <c r="AQ20" s="15"/>
       <c r="AR20" s="15"/>
     </row>
-    <row r="21" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
@@ -2297,7 +2300,7 @@
       </c>
       <c r="J21" s="33"/>
       <c r="K21" s="19" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
@@ -2333,7 +2336,7 @@
       <c r="AQ21" s="15"/>
       <c r="AR21" s="15"/>
     </row>
-    <row r="22" spans="1:44" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:44" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -2359,7 +2362,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
@@ -2395,12 +2398,12 @@
       <c r="AQ22" s="15"/>
       <c r="AR22" s="15"/>
     </row>
-    <row r="23" spans="1:44" outlineLevel="3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:44" outlineLevel="3" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="23" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="E23" s="16">
         <v>1</v>
@@ -2421,7 +2424,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
@@ -2457,11 +2460,11 @@
       <c r="AQ23" s="15"/>
       <c r="AR23" s="15"/>
     </row>
-    <row r="24" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="9"/>
       <c r="C24" s="18" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10">
@@ -2483,7 +2486,7 @@
         <v>1</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
@@ -2519,11 +2522,11 @@
       <c r="AQ24" s="15"/>
       <c r="AR24" s="15"/>
     </row>
-    <row r="25" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="9"/>
       <c r="C25" s="18" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10">
@@ -2545,7 +2548,7 @@
         <v>1</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
@@ -2581,11 +2584,11 @@
       <c r="AQ25" s="15"/>
       <c r="AR25" s="15"/>
     </row>
-    <row r="26" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9"/>
       <c r="C26" s="18" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10">
@@ -2607,7 +2610,7 @@
         <v>1</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
@@ -2643,11 +2646,11 @@
       <c r="AQ26" s="15"/>
       <c r="AR26" s="15"/>
     </row>
-    <row r="27" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="9"/>
       <c r="C27" s="18" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10">
@@ -2669,7 +2672,7 @@
         <v>1</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
@@ -2705,11 +2708,11 @@
       <c r="AQ27" s="15"/>
       <c r="AR27" s="15"/>
     </row>
-    <row r="28" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9"/>
       <c r="C28" s="18" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10">
@@ -2731,7 +2734,7 @@
         <v>1</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
@@ -2767,10 +2770,10 @@
       <c r="AQ28" s="15"/>
       <c r="AR28" s="15"/>
     </row>
-    <row r="29" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="18" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="10"/>
@@ -2823,11 +2826,11 @@
       <c r="AQ29" s="15"/>
       <c r="AR29" s="15"/>
     </row>
-    <row r="30" spans="1:44" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:44" ht="16.5" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="9"/>
       <c r="C30" s="18" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10">
@@ -2849,7 +2852,7 @@
         <v>1</v>
       </c>
       <c r="K30" s="24" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
@@ -2885,11 +2888,11 @@
       <c r="AQ30" s="15"/>
       <c r="AR30" s="15"/>
     </row>
-    <row r="31" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="9"/>
       <c r="C31" s="18" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10">
@@ -2911,7 +2914,7 @@
         <v>1</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
@@ -2947,11 +2950,11 @@
       <c r="AQ31" s="15"/>
       <c r="AR31" s="15"/>
     </row>
-    <row r="32" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="18" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10">
@@ -2973,7 +2976,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
@@ -3009,11 +3012,11 @@
       <c r="AQ32" s="15"/>
       <c r="AR32" s="15"/>
     </row>
-    <row r="33" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="9"/>
       <c r="C33" s="18" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D33" s="10"/>
       <c r="E33" s="10">
@@ -3035,7 +3038,7 @@
         <v>1</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
@@ -3071,15 +3074,15 @@
       <c r="AQ33" s="15"/>
       <c r="AR33" s="15"/>
     </row>
-    <row r="34" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="9"/>
       <c r="C34" s="18" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F34" s="11">
         <v>43004</v>
@@ -3097,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
@@ -3133,11 +3136,11 @@
       <c r="AQ34" s="15"/>
       <c r="AR34" s="15"/>
     </row>
-    <row r="35" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="9"/>
       <c r="C35" s="18" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10">
@@ -3159,7 +3162,7 @@
         <v>1</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
@@ -3195,10 +3198,10 @@
       <c r="AQ35" s="15"/>
       <c r="AR35" s="15"/>
     </row>
-    <row r="36" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="18" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="10"/>
@@ -3221,7 +3224,7 @@
         <v>1</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
@@ -3257,9 +3260,9 @@
       <c r="AQ36" s="15"/>
       <c r="AR36" s="15"/>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -3313,10 +3316,10 @@
       <c r="AQ37" s="15"/>
       <c r="AR37" s="15"/>
     </row>
-    <row r="38" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="18" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C38" s="9"/>
       <c r="D38" s="10"/>
@@ -3335,7 +3338,7 @@
       </c>
       <c r="J38" s="33"/>
       <c r="K38" s="19" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
@@ -3371,11 +3374,11 @@
       <c r="AQ38" s="15"/>
       <c r="AR38" s="15"/>
     </row>
-    <row r="39" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="9"/>
       <c r="C39" s="18" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10">
@@ -3397,7 +3400,7 @@
         <v>1</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
@@ -3433,11 +3436,11 @@
       <c r="AQ39" s="15"/>
       <c r="AR39" s="15"/>
     </row>
-    <row r="40" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="9"/>
       <c r="C40" s="18" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10">
@@ -3459,7 +3462,7 @@
         <v>1</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
@@ -3495,10 +3498,10 @@
       <c r="AQ40" s="15"/>
       <c r="AR40" s="15"/>
     </row>
-    <row r="41" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="18" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="10"/>
@@ -3521,7 +3524,7 @@
         <v>1</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
@@ -3557,10 +3560,10 @@
       <c r="AQ41" s="15"/>
       <c r="AR41" s="15"/>
     </row>
-    <row r="42" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="18" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="10"/>
@@ -3583,7 +3586,7 @@
         <v>1</v>
       </c>
       <c r="K42" s="19" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
@@ -3619,10 +3622,10 @@
       <c r="AQ42" s="15"/>
       <c r="AR42" s="15"/>
     </row>
-    <row r="43" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="18" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="C43" s="9"/>
       <c r="D43" s="10"/>
@@ -3645,7 +3648,7 @@
         <v>1</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
@@ -3681,28 +3684,28 @@
       <c r="AQ43" s="15"/>
       <c r="AR43" s="15"/>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A44" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="B44" s="9"/>
+    <row r="44" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="18"/>
       <c r="C44" s="9"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
       <c r="F44" s="11">
+        <v>43052</v>
+      </c>
+      <c r="G44" s="11">
+        <v>43052</v>
+      </c>
+      <c r="H44" s="11">
         <v>43080</v>
       </c>
-      <c r="G44" s="11">
+      <c r="I44" s="11">
         <v>43080</v>
       </c>
-      <c r="H44" s="11">
-        <v>43174</v>
-      </c>
-      <c r="I44" s="11">
-        <v>43174</v>
-      </c>
       <c r="J44" s="33"/>
-      <c r="K44" s="14"/>
+      <c r="K44" s="19"/>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
@@ -3716,20 +3719,20 @@
       <c r="V44" s="15"/>
       <c r="W44" s="15"/>
       <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
+      <c r="Y44" s="29"/>
+      <c r="Z44" s="29"/>
       <c r="AA44" s="29"/>
-      <c r="AB44" s="29"/>
-      <c r="AC44" s="29"/>
-      <c r="AD44" s="29"/>
-      <c r="AE44" s="29"/>
-      <c r="AF44" s="29"/>
-      <c r="AG44" s="29"/>
-      <c r="AH44" s="29"/>
-      <c r="AI44" s="29"/>
-      <c r="AJ44" s="29"/>
-      <c r="AK44" s="29"/>
-      <c r="AL44" s="29"/>
+      <c r="AB44" s="15"/>
+      <c r="AC44" s="15"/>
+      <c r="AD44" s="15"/>
+      <c r="AE44" s="15"/>
+      <c r="AF44" s="15"/>
+      <c r="AG44" s="15"/>
+      <c r="AH44" s="15"/>
+      <c r="AI44" s="15"/>
+      <c r="AJ44" s="15"/>
+      <c r="AK44" s="15"/>
+      <c r="AL44" s="15"/>
       <c r="AM44" s="15"/>
       <c r="AN44" s="15"/>
       <c r="AO44" s="15"/>
@@ -3737,28 +3740,34 @@
       <c r="AQ44" s="15"/>
       <c r="AR44" s="15"/>
     </row>
-    <row r="45" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
-      <c r="B45" s="9" t="s">
-        <v>13</v>
+      <c r="B45" s="18" t="s">
+        <v>69</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
+      <c r="E45" s="10">
+        <v>27</v>
+      </c>
       <c r="F45" s="11">
+        <v>43052</v>
+      </c>
+      <c r="G45" s="11">
+        <v>43052</v>
+      </c>
+      <c r="H45" s="11">
         <v>43080</v>
       </c>
-      <c r="G45" s="11">
+      <c r="I45" s="11">
         <v>43080</v>
       </c>
-      <c r="H45" s="11">
-        <v>43084</v>
-      </c>
-      <c r="I45" s="11">
-        <v>43084</v>
-      </c>
-      <c r="J45" s="33"/>
-      <c r="K45" s="19"/>
+      <c r="J45" s="17">
+        <v>1</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
@@ -3793,33 +3802,33 @@
       <c r="AQ45" s="15"/>
       <c r="AR45" s="15"/>
     </row>
-    <row r="46" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="B46" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C46" s="9"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F46" s="11">
+        <v>43052</v>
+      </c>
+      <c r="G46" s="11">
+        <v>43052</v>
+      </c>
+      <c r="H46" s="11">
         <v>43080</v>
       </c>
-      <c r="G46" s="11">
+      <c r="I46" s="11">
         <v>43080</v>
       </c>
-      <c r="H46" s="11">
-        <v>43084</v>
-      </c>
-      <c r="I46" s="11">
-        <v>43084</v>
-      </c>
       <c r="J46" s="17">
         <v>1</v>
       </c>
-      <c r="K46" s="14" t="s">
-        <v>91</v>
+      <c r="K46" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
@@ -3855,11 +3864,11 @@
       <c r="AQ46" s="15"/>
       <c r="AR46" s="15"/>
     </row>
-    <row r="47" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="8"/>
-      <c r="B47" s="18" t="s">
-        <v>66</v>
-      </c>
+    <row r="47" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="9"/>
       <c r="C47" s="9"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
@@ -3870,15 +3879,13 @@
         <v>43080</v>
       </c>
       <c r="H47" s="11">
-        <v>43125</v>
+        <v>43174</v>
       </c>
       <c r="I47" s="11">
-        <v>43125</v>
+        <v>43174</v>
       </c>
       <c r="J47" s="33"/>
-      <c r="K47" s="19" t="s">
-        <v>90</v>
-      </c>
+      <c r="K47" s="14"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
       <c r="N47" s="15"/>
@@ -3899,13 +3906,13 @@
       <c r="AC47" s="29"/>
       <c r="AD47" s="29"/>
       <c r="AE47" s="29"/>
-      <c r="AF47" s="15"/>
-      <c r="AG47" s="15"/>
-      <c r="AH47" s="15"/>
-      <c r="AI47" s="15"/>
-      <c r="AJ47" s="15"/>
-      <c r="AK47" s="15"/>
-      <c r="AL47" s="15"/>
+      <c r="AF47" s="29"/>
+      <c r="AG47" s="29"/>
+      <c r="AH47" s="29"/>
+      <c r="AI47" s="29"/>
+      <c r="AJ47" s="29"/>
+      <c r="AK47" s="29"/>
+      <c r="AL47" s="29"/>
       <c r="AM47" s="15"/>
       <c r="AN47" s="15"/>
       <c r="AO47" s="15"/>
@@ -3913,16 +3920,14 @@
       <c r="AQ47" s="15"/>
       <c r="AR47" s="15"/>
     </row>
-    <row r="48" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="9" t="s">
-        <v>94</v>
-      </c>
+      <c r="B48" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="9"/>
       <c r="D48" s="10"/>
-      <c r="E48" s="10">
-        <v>12</v>
-      </c>
+      <c r="E48" s="10"/>
       <c r="F48" s="11">
         <v>43080</v>
       </c>
@@ -3930,17 +3935,13 @@
         <v>43080</v>
       </c>
       <c r="H48" s="11">
-        <v>43125</v>
+        <v>43084</v>
       </c>
       <c r="I48" s="11">
-        <v>43125</v>
-      </c>
-      <c r="J48" s="17">
-        <v>1</v>
-      </c>
-      <c r="K48" s="19" t="s">
-        <v>37</v>
-      </c>
+        <v>43084</v>
+      </c>
+      <c r="J48" s="33"/>
+      <c r="K48" s="19"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
       <c r="N48" s="15"/>
@@ -3975,15 +3976,15 @@
       <c r="AQ48" s="15"/>
       <c r="AR48" s="15"/>
     </row>
-    <row r="49" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
-      <c r="B49" s="18"/>
+      <c r="B49" s="9"/>
       <c r="C49" s="9" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="D49" s="10"/>
       <c r="E49" s="10">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F49" s="11">
         <v>43080</v>
@@ -3992,16 +3993,16 @@
         <v>43080</v>
       </c>
       <c r="H49" s="11">
-        <v>43125</v>
+        <v>43084</v>
       </c>
       <c r="I49" s="11">
-        <v>43125</v>
+        <v>43084</v>
       </c>
       <c r="J49" s="17">
         <v>1</v>
       </c>
-      <c r="K49" s="19" t="s">
-        <v>34</v>
+      <c r="K49" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
@@ -4037,16 +4038,14 @@
       <c r="AQ49" s="15"/>
       <c r="AR49" s="15"/>
     </row>
-    <row r="50" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
-      <c r="B50" s="18"/>
-      <c r="C50" s="9" t="s">
-        <v>96</v>
-      </c>
+      <c r="B50" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="9"/>
       <c r="D50" s="10"/>
-      <c r="E50" s="10">
-        <v>7</v>
-      </c>
+      <c r="E50" s="10"/>
       <c r="F50" s="11">
         <v>43080</v>
       </c>
@@ -4059,11 +4058,9 @@
       <c r="I50" s="11">
         <v>43125</v>
       </c>
-      <c r="J50" s="17">
-        <v>1</v>
-      </c>
+      <c r="J50" s="33"/>
       <c r="K50" s="19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
@@ -4080,11 +4077,11 @@
       <c r="X50" s="15"/>
       <c r="Y50" s="15"/>
       <c r="Z50" s="15"/>
-      <c r="AA50" s="15"/>
-      <c r="AB50" s="15"/>
-      <c r="AC50" s="15"/>
-      <c r="AD50" s="15"/>
-      <c r="AE50" s="15"/>
+      <c r="AA50" s="29"/>
+      <c r="AB50" s="29"/>
+      <c r="AC50" s="29"/>
+      <c r="AD50" s="29"/>
+      <c r="AE50" s="29"/>
       <c r="AF50" s="15"/>
       <c r="AG50" s="15"/>
       <c r="AH50" s="15"/>
@@ -4099,29 +4096,33 @@
       <c r="AQ50" s="15"/>
       <c r="AR50" s="15"/>
     </row>
-    <row r="51" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
-      <c r="B51" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C51" s="9"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
+      <c r="E51" s="10">
+        <v>12</v>
+      </c>
       <c r="F51" s="11">
-        <v>43126</v>
+        <v>43080</v>
       </c>
       <c r="G51" s="11">
-        <v>43126</v>
+        <v>43080</v>
       </c>
       <c r="H51" s="11">
-        <v>43131</v>
+        <v>43125</v>
       </c>
       <c r="I51" s="11">
-        <v>43131</v>
-      </c>
-      <c r="J51" s="33"/>
+        <v>43125</v>
+      </c>
+      <c r="J51" s="17">
+        <v>1</v>
+      </c>
       <c r="K51" s="19" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
@@ -4143,7 +4144,7 @@
       <c r="AC51" s="15"/>
       <c r="AD51" s="15"/>
       <c r="AE51" s="15"/>
-      <c r="AF51" s="29"/>
+      <c r="AF51" s="15"/>
       <c r="AG51" s="15"/>
       <c r="AH51" s="15"/>
       <c r="AI51" s="15"/>
@@ -4157,33 +4158,33 @@
       <c r="AQ51" s="15"/>
       <c r="AR51" s="15"/>
     </row>
-    <row r="52" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
-      <c r="B52" s="9"/>
+      <c r="B52" s="18"/>
       <c r="C52" s="9" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="10">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F52" s="11">
-        <v>43126</v>
+        <v>43080</v>
       </c>
       <c r="G52" s="11">
-        <v>43126</v>
+        <v>43080</v>
       </c>
       <c r="H52" s="11">
-        <v>43131</v>
+        <v>43125</v>
       </c>
       <c r="I52" s="11">
-        <v>43131</v>
+        <v>43125</v>
       </c>
       <c r="J52" s="17">
         <v>1</v>
       </c>
       <c r="K52" s="19" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
@@ -4219,33 +4220,33 @@
       <c r="AQ52" s="15"/>
       <c r="AR52" s="15"/>
     </row>
-    <row r="53" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
-      <c r="B53" s="9"/>
+      <c r="B53" s="18"/>
       <c r="C53" s="9" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F53" s="11">
-        <v>43126</v>
+        <v>43080</v>
       </c>
       <c r="G53" s="11">
-        <v>43126</v>
+        <v>43080</v>
       </c>
       <c r="H53" s="11">
-        <v>43131</v>
+        <v>43125</v>
       </c>
       <c r="I53" s="11">
-        <v>43131</v>
+        <v>43125</v>
       </c>
       <c r="J53" s="17">
         <v>1</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
@@ -4281,16 +4282,14 @@
       <c r="AQ53" s="15"/>
       <c r="AR53" s="15"/>
     </row>
-    <row r="54" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="9" t="s">
-        <v>18</v>
-      </c>
+      <c r="B54" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="9"/>
       <c r="D54" s="10"/>
-      <c r="E54" s="10">
-        <v>1</v>
-      </c>
+      <c r="E54" s="10"/>
       <c r="F54" s="11">
         <v>43126</v>
       </c>
@@ -4303,11 +4302,9 @@
       <c r="I54" s="11">
         <v>43131</v>
       </c>
-      <c r="J54" s="17">
-        <v>1</v>
-      </c>
+      <c r="J54" s="33"/>
       <c r="K54" s="19" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -4329,7 +4326,7 @@
       <c r="AC54" s="15"/>
       <c r="AD54" s="15"/>
       <c r="AE54" s="15"/>
-      <c r="AF54" s="15"/>
+      <c r="AF54" s="29"/>
       <c r="AG54" s="15"/>
       <c r="AH54" s="15"/>
       <c r="AI54" s="15"/>
@@ -4343,11 +4340,11 @@
       <c r="AQ54" s="15"/>
       <c r="AR54" s="15"/>
     </row>
-    <row r="55" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="10">
@@ -4369,7 +4366,7 @@
         <v>1</v>
       </c>
       <c r="K55" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
@@ -4405,33 +4402,33 @@
       <c r="AQ55" s="15"/>
       <c r="AR55" s="15"/>
     </row>
-    <row r="56" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
-      <c r="B56" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="D56" s="10"/>
       <c r="E56" s="10">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F56" s="11">
+        <v>43126</v>
+      </c>
+      <c r="G56" s="11">
+        <v>43126</v>
+      </c>
+      <c r="H56" s="11">
         <v>43131</v>
       </c>
-      <c r="G56" s="11">
+      <c r="I56" s="11">
         <v>43131</v>
       </c>
-      <c r="H56" s="11">
-        <v>43154</v>
-      </c>
-      <c r="I56" s="11">
-        <v>43184</v>
-      </c>
-      <c r="J56" s="32">
+      <c r="J56" s="17">
         <v>1</v>
       </c>
       <c r="K56" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
@@ -4453,10 +4450,10 @@
       <c r="AC56" s="15"/>
       <c r="AD56" s="15"/>
       <c r="AE56" s="15"/>
-      <c r="AF56" s="29"/>
-      <c r="AG56" s="29"/>
-      <c r="AH56" s="29"/>
-      <c r="AI56" s="29"/>
+      <c r="AF56" s="15"/>
+      <c r="AG56" s="15"/>
+      <c r="AH56" s="15"/>
+      <c r="AI56" s="15"/>
       <c r="AJ56" s="15"/>
       <c r="AK56" s="15"/>
       <c r="AL56" s="15"/>
@@ -4467,33 +4464,33 @@
       <c r="AQ56" s="15"/>
       <c r="AR56" s="15"/>
     </row>
-    <row r="57" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
-      <c r="B57" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="D57" s="10"/>
       <c r="E57" s="10">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F57" s="11">
-        <v>43155</v>
+        <v>43126</v>
       </c>
       <c r="G57" s="11">
-        <v>43185</v>
+        <v>43126</v>
       </c>
       <c r="H57" s="11">
-        <v>43161</v>
-      </c>
-      <c r="I57" s="12">
-        <v>43186</v>
-      </c>
-      <c r="J57" s="32">
+        <v>43131</v>
+      </c>
+      <c r="I57" s="11">
+        <v>43131</v>
+      </c>
+      <c r="J57" s="17">
         <v>1</v>
       </c>
       <c r="K57" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
@@ -4519,8 +4516,8 @@
       <c r="AG57" s="15"/>
       <c r="AH57" s="15"/>
       <c r="AI57" s="15"/>
-      <c r="AJ57" s="29"/>
-      <c r="AK57" s="29"/>
+      <c r="AJ57" s="15"/>
+      <c r="AK57" s="15"/>
       <c r="AL57" s="15"/>
       <c r="AM57" s="15"/>
       <c r="AN57" s="15"/>
@@ -4529,33 +4526,33 @@
       <c r="AQ57" s="15"/>
       <c r="AR57" s="15"/>
     </row>
-    <row r="58" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
-      <c r="B58" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9" t="s">
+        <v>82</v>
+      </c>
       <c r="D58" s="10"/>
       <c r="E58" s="10">
         <v>1</v>
       </c>
       <c r="F58" s="11">
-        <v>43173</v>
+        <v>43126</v>
       </c>
       <c r="G58" s="11">
-        <v>43187</v>
+        <v>43126</v>
       </c>
       <c r="H58" s="11">
-        <v>43174</v>
-      </c>
-      <c r="I58" s="12">
-        <v>43194</v>
-      </c>
-      <c r="J58" s="32">
+        <v>43131</v>
+      </c>
+      <c r="I58" s="11">
+        <v>43131</v>
+      </c>
+      <c r="J58" s="17">
         <v>1</v>
       </c>
       <c r="K58" s="19" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -4583,7 +4580,7 @@
       <c r="AI58" s="15"/>
       <c r="AJ58" s="15"/>
       <c r="AK58" s="15"/>
-      <c r="AL58" s="29"/>
+      <c r="AL58" s="15"/>
       <c r="AM58" s="15"/>
       <c r="AN58" s="15"/>
       <c r="AO58" s="15"/>
@@ -4591,28 +4588,34 @@
       <c r="AQ58" s="15"/>
       <c r="AR58" s="15"/>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A59" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" s="9"/>
+    <row r="59" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="18" t="s">
+        <v>83</v>
+      </c>
       <c r="C59" s="9"/>
       <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
+      <c r="E59" s="10">
+        <v>15</v>
+      </c>
       <c r="F59" s="11">
-        <v>43190</v>
+        <v>43131</v>
       </c>
       <c r="G59" s="11">
-        <v>43192</v>
+        <v>43131</v>
       </c>
       <c r="H59" s="11">
-        <v>43194</v>
-      </c>
-      <c r="I59" s="12">
-        <v>43202</v>
-      </c>
-      <c r="J59" s="34"/>
-      <c r="K59" s="19"/>
+        <v>43154</v>
+      </c>
+      <c r="I59" s="11">
+        <v>43184</v>
+      </c>
+      <c r="J59" s="32">
+        <v>1</v>
+      </c>
+      <c r="K59" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
       <c r="N59" s="15"/>
@@ -4633,47 +4636,47 @@
       <c r="AC59" s="15"/>
       <c r="AD59" s="15"/>
       <c r="AE59" s="15"/>
-      <c r="AF59" s="15"/>
-      <c r="AG59" s="15"/>
-      <c r="AH59" s="15"/>
-      <c r="AI59" s="15"/>
+      <c r="AF59" s="29"/>
+      <c r="AG59" s="29"/>
+      <c r="AH59" s="29"/>
+      <c r="AI59" s="29"/>
       <c r="AJ59" s="15"/>
       <c r="AK59" s="15"/>
       <c r="AL59" s="15"/>
       <c r="AM59" s="15"/>
-      <c r="AN59" s="29"/>
-      <c r="AO59" s="29"/>
+      <c r="AN59" s="15"/>
+      <c r="AO59" s="15"/>
       <c r="AP59" s="15"/>
       <c r="AQ59" s="15"/>
       <c r="AR59" s="15"/>
     </row>
-    <row r="60" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
-      <c r="B60" s="9" t="s">
-        <v>19</v>
+      <c r="B60" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="10"/>
       <c r="E60" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F60" s="11">
-        <v>43190</v>
+        <v>43155</v>
       </c>
       <c r="G60" s="11">
-        <v>43192</v>
+        <v>43185</v>
       </c>
       <c r="H60" s="11">
-        <v>43192</v>
+        <v>43161</v>
       </c>
       <c r="I60" s="12">
-        <v>43202</v>
+        <v>43186</v>
       </c>
       <c r="J60" s="32">
         <v>1</v>
       </c>
       <c r="K60" s="19" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
@@ -4699,8 +4702,8 @@
       <c r="AG60" s="15"/>
       <c r="AH60" s="15"/>
       <c r="AI60" s="15"/>
-      <c r="AJ60" s="15"/>
-      <c r="AK60" s="15"/>
+      <c r="AJ60" s="29"/>
+      <c r="AK60" s="29"/>
       <c r="AL60" s="15"/>
       <c r="AM60" s="15"/>
       <c r="AN60" s="15"/>
@@ -4709,33 +4712,33 @@
       <c r="AQ60" s="15"/>
       <c r="AR60" s="15"/>
     </row>
-    <row r="61" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
-      <c r="B61" s="9" t="s">
-        <v>20</v>
+      <c r="B61" s="18" t="s">
+        <v>85</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="10"/>
       <c r="E61" s="10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F61" s="11">
-        <v>43190</v>
+        <v>43173</v>
       </c>
       <c r="G61" s="11">
-        <v>43192</v>
+        <v>43187</v>
       </c>
       <c r="H61" s="11">
+        <v>43174</v>
+      </c>
+      <c r="I61" s="12">
         <v>43194</v>
       </c>
-      <c r="I61" s="12">
-        <v>43202</v>
-      </c>
       <c r="J61" s="32">
         <v>1</v>
       </c>
       <c r="K61" s="19" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
@@ -4763,7 +4766,7 @@
       <c r="AI61" s="15"/>
       <c r="AJ61" s="15"/>
       <c r="AK61" s="15"/>
-      <c r="AL61" s="15"/>
+      <c r="AL61" s="29"/>
       <c r="AM61" s="15"/>
       <c r="AN61" s="15"/>
       <c r="AO61" s="15"/>
@@ -4771,11 +4774,11 @@
       <c r="AQ61" s="15"/>
       <c r="AR61" s="15"/>
     </row>
-    <row r="62" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="8"/>
-      <c r="B62" s="9" t="s">
-        <v>24</v>
-      </c>
+    <row r="62" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A62" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" s="9"/>
       <c r="C62" s="9"/>
       <c r="D62" s="10"/>
       <c r="E62" s="10"/>
@@ -4783,18 +4786,16 @@
         <v>43190</v>
       </c>
       <c r="G62" s="11">
-        <v>43211</v>
+        <v>43192</v>
       </c>
       <c r="H62" s="11">
         <v>43194</v>
       </c>
-      <c r="I62" s="11">
-        <v>43211</v>
+      <c r="I62" s="12">
+        <v>43202</v>
       </c>
       <c r="J62" s="34"/>
-      <c r="K62" s="19" t="s">
-        <v>89</v>
-      </c>
+      <c r="K62" s="19"/>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
@@ -4823,39 +4824,39 @@
       <c r="AK62" s="15"/>
       <c r="AL62" s="15"/>
       <c r="AM62" s="15"/>
-      <c r="AN62" s="15"/>
-      <c r="AO62" s="15"/>
+      <c r="AN62" s="29"/>
+      <c r="AO62" s="29"/>
       <c r="AP62" s="15"/>
       <c r="AQ62" s="15"/>
       <c r="AR62" s="15"/>
     </row>
-    <row r="63" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9" t="s">
-        <v>25</v>
-      </c>
+      <c r="B63" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C63" s="9"/>
       <c r="D63" s="10"/>
       <c r="E63" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F63" s="11">
         <v>43190</v>
       </c>
       <c r="G63" s="11">
-        <v>43211</v>
+        <v>43192</v>
       </c>
       <c r="H63" s="11">
-        <v>43194</v>
-      </c>
-      <c r="I63" s="11">
-        <v>43211</v>
+        <v>43192</v>
+      </c>
+      <c r="I63" s="12">
+        <v>43202</v>
       </c>
       <c r="J63" s="32">
         <v>1</v>
       </c>
       <c r="K63" s="19" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
@@ -4891,33 +4892,33 @@
       <c r="AQ63" s="15"/>
       <c r="AR63" s="15"/>
     </row>
-    <row r="64" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="B64" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="9"/>
       <c r="D64" s="10"/>
       <c r="E64" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F64" s="11">
         <v>43190</v>
       </c>
       <c r="G64" s="11">
-        <v>43211</v>
+        <v>43192</v>
       </c>
       <c r="H64" s="11">
         <v>43194</v>
       </c>
-      <c r="I64" s="11">
-        <v>43211</v>
+      <c r="I64" s="12">
+        <v>43202</v>
       </c>
       <c r="J64" s="32">
         <v>1</v>
       </c>
       <c r="K64" s="19" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
@@ -4953,26 +4954,30 @@
       <c r="AQ64" s="15"/>
       <c r="AR64" s="15"/>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A65" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B65" s="9"/>
+    <row r="65" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="8"/>
+      <c r="B65" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="C65" s="9"/>
       <c r="D65" s="10"/>
       <c r="E65" s="10"/>
       <c r="F65" s="11">
-        <v>43073</v>
+        <v>43190</v>
       </c>
       <c r="G65" s="11">
-        <v>43073</v>
+        <v>43211</v>
       </c>
       <c r="H65" s="11">
-        <v>43217</v>
-      </c>
-      <c r="I65" s="12"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="19"/>
+        <v>43194</v>
+      </c>
+      <c r="I65" s="11">
+        <v>43211</v>
+      </c>
+      <c r="J65" s="34"/>
+      <c r="K65" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
@@ -4988,52 +4993,52 @@
       <c r="X65" s="15"/>
       <c r="Y65" s="15"/>
       <c r="Z65" s="15"/>
-      <c r="AA65" s="29"/>
-      <c r="AB65" s="29"/>
-      <c r="AC65" s="29"/>
-      <c r="AD65" s="29"/>
-      <c r="AE65" s="29"/>
-      <c r="AF65" s="29"/>
-      <c r="AG65" s="29"/>
-      <c r="AH65" s="29"/>
-      <c r="AI65" s="29"/>
-      <c r="AJ65" s="29"/>
-      <c r="AK65" s="29"/>
-      <c r="AL65" s="29"/>
-      <c r="AM65" s="29"/>
-      <c r="AN65" s="29"/>
-      <c r="AO65" s="29"/>
-      <c r="AP65" s="29"/>
-      <c r="AQ65" s="29"/>
-      <c r="AR65" s="29"/>
-    </row>
-    <row r="66" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="AA65" s="15"/>
+      <c r="AB65" s="15"/>
+      <c r="AC65" s="15"/>
+      <c r="AD65" s="15"/>
+      <c r="AE65" s="15"/>
+      <c r="AF65" s="15"/>
+      <c r="AG65" s="15"/>
+      <c r="AH65" s="15"/>
+      <c r="AI65" s="15"/>
+      <c r="AJ65" s="15"/>
+      <c r="AK65" s="15"/>
+      <c r="AL65" s="15"/>
+      <c r="AM65" s="15"/>
+      <c r="AN65" s="15"/>
+      <c r="AO65" s="15"/>
+      <c r="AP65" s="15"/>
+      <c r="AQ65" s="15"/>
+      <c r="AR65" s="15"/>
+    </row>
+    <row r="66" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A66" s="8"/>
-      <c r="B66" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="C66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9" t="s">
+        <v>89</v>
+      </c>
       <c r="D66" s="10"/>
       <c r="E66" s="10">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F66" s="11">
-        <v>43161</v>
+        <v>43190</v>
       </c>
       <c r="G66" s="11">
-        <v>43161</v>
+        <v>43211</v>
       </c>
       <c r="H66" s="11">
-        <v>43203</v>
-      </c>
-      <c r="I66" s="12">
-        <v>43203</v>
-      </c>
-      <c r="J66" s="17">
+        <v>43194</v>
+      </c>
+      <c r="I66" s="11">
+        <v>43211</v>
+      </c>
+      <c r="J66" s="32">
         <v>1</v>
       </c>
       <c r="K66" s="19" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
@@ -5069,27 +5074,33 @@
       <c r="AQ66" s="15"/>
       <c r="AR66" s="15"/>
     </row>
-    <row r="67" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
-      <c r="B67" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C67" s="9"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
+      <c r="E67" s="10">
+        <v>1</v>
+      </c>
       <c r="F67" s="11">
-        <v>43073</v>
+        <v>43190</v>
       </c>
       <c r="G67" s="11">
-        <v>43073</v>
+        <v>43211</v>
       </c>
       <c r="H67" s="11">
-        <v>43217</v>
-      </c>
-      <c r="I67" s="12"/>
-      <c r="J67" s="13"/>
+        <v>43194</v>
+      </c>
+      <c r="I67" s="11">
+        <v>43211</v>
+      </c>
+      <c r="J67" s="32">
+        <v>1</v>
+      </c>
       <c r="K67" s="19" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="L67" s="15"/>
       <c r="M67" s="15"/>
@@ -5125,16 +5136,14 @@
       <c r="AQ67" s="15"/>
       <c r="AR67" s="15"/>
     </row>
-    <row r="68" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
-      <c r="A68" s="8"/>
+    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A68" s="8" t="s">
+        <v>91</v>
+      </c>
       <c r="B68" s="9"/>
-      <c r="C68" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="C68" s="9"/>
       <c r="D68" s="10"/>
-      <c r="E68" s="10">
-        <v>2</v>
-      </c>
+      <c r="E68" s="10"/>
       <c r="F68" s="11">
         <v>43073</v>
       </c>
@@ -5142,17 +5151,11 @@
         <v>43073</v>
       </c>
       <c r="H68" s="11">
-        <v>43077</v>
-      </c>
-      <c r="I68" s="11">
-        <v>43077</v>
-      </c>
-      <c r="J68" s="17">
-        <v>1</v>
-      </c>
-      <c r="K68" s="19" t="s">
-        <v>35</v>
-      </c>
+        <v>43217</v>
+      </c>
+      <c r="I68" s="12"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="19"/>
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
@@ -5168,48 +5171,52 @@
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
       <c r="Z68" s="15"/>
-      <c r="AA68" s="15"/>
-      <c r="AB68" s="15"/>
-      <c r="AC68" s="15"/>
-      <c r="AD68" s="15"/>
-      <c r="AE68" s="15"/>
-      <c r="AF68" s="15"/>
-      <c r="AG68" s="15"/>
-      <c r="AH68" s="15"/>
-      <c r="AI68" s="15"/>
-      <c r="AJ68" s="15"/>
-      <c r="AK68" s="15"/>
-      <c r="AL68" s="15"/>
-      <c r="AM68" s="15"/>
-      <c r="AN68" s="15"/>
-      <c r="AO68" s="15"/>
-      <c r="AP68" s="15"/>
-      <c r="AQ68" s="15"/>
-      <c r="AR68" s="15"/>
-    </row>
-    <row r="69" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+      <c r="AA68" s="29"/>
+      <c r="AB68" s="29"/>
+      <c r="AC68" s="29"/>
+      <c r="AD68" s="29"/>
+      <c r="AE68" s="29"/>
+      <c r="AF68" s="29"/>
+      <c r="AG68" s="29"/>
+      <c r="AH68" s="29"/>
+      <c r="AI68" s="29"/>
+      <c r="AJ68" s="29"/>
+      <c r="AK68" s="29"/>
+      <c r="AL68" s="29"/>
+      <c r="AM68" s="29"/>
+      <c r="AN68" s="29"/>
+      <c r="AO68" s="29"/>
+      <c r="AP68" s="29"/>
+      <c r="AQ68" s="29"/>
+      <c r="AR68" s="29"/>
+    </row>
+    <row r="69" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="B69" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="9"/>
       <c r="D69" s="10"/>
       <c r="E69" s="10">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F69" s="11">
-        <v>43206</v>
+        <v>43161</v>
       </c>
       <c r="G69" s="11">
-        <v>43206</v>
+        <v>43161</v>
       </c>
       <c r="H69" s="11">
-        <v>43217</v>
-      </c>
-      <c r="I69" s="12"/>
-      <c r="J69" s="13"/>
+        <v>43203</v>
+      </c>
+      <c r="I69" s="12">
+        <v>43203</v>
+      </c>
+      <c r="J69" s="17">
+        <v>1</v>
+      </c>
       <c r="K69" s="19" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
@@ -5245,21 +5252,19 @@
       <c r="AQ69" s="15"/>
       <c r="AR69" s="15"/>
     </row>
-    <row r="70" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:44" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
-      <c r="B70" s="9"/>
-      <c r="C70" s="18" t="s">
-        <v>61</v>
-      </c>
+      <c r="B70" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="9"/>
       <c r="D70" s="10"/>
-      <c r="E70" s="10">
-        <v>3</v>
-      </c>
+      <c r="E70" s="10"/>
       <c r="F70" s="11">
-        <v>43206</v>
+        <v>43073</v>
       </c>
       <c r="G70" s="11">
-        <v>43206</v>
+        <v>43073</v>
       </c>
       <c r="H70" s="11">
         <v>43217</v>
@@ -5267,7 +5272,7 @@
       <c r="I70" s="12"/>
       <c r="J70" s="13"/>
       <c r="K70" s="19" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="L70" s="15"/>
       <c r="M70" s="15"/>
@@ -5303,33 +5308,33 @@
       <c r="AQ70" s="15"/>
       <c r="AR70" s="15"/>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A71" s="8" t="s">
-        <v>82</v>
-      </c>
+    <row r="71" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
       <c r="B71" s="9"/>
-      <c r="C71" s="9"/>
+      <c r="C71" s="9" t="s">
+        <v>94</v>
+      </c>
       <c r="D71" s="10"/>
       <c r="E71" s="10">
         <v>2</v>
       </c>
       <c r="F71" s="11">
-        <v>43199</v>
+        <v>43073</v>
       </c>
       <c r="G71" s="11">
-        <v>43199</v>
+        <v>43073</v>
       </c>
       <c r="H71" s="11">
-        <v>43203</v>
+        <v>43077</v>
       </c>
       <c r="I71" s="11">
-        <v>43202</v>
+        <v>43077</v>
       </c>
       <c r="J71" s="17">
         <v>1</v>
       </c>
-      <c r="K71" s="14" t="s">
-        <v>33</v>
+      <c r="K71" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="L71" s="15"/>
       <c r="M71" s="15"/>
@@ -5341,7 +5346,7 @@
       <c r="S71" s="15"/>
       <c r="T71" s="15"/>
       <c r="U71" s="15"/>
-      <c r="V71" s="29"/>
+      <c r="V71" s="15"/>
       <c r="W71" s="15"/>
       <c r="X71" s="15"/>
       <c r="Y71" s="15"/>
@@ -5365,28 +5370,30 @@
       <c r="AQ71" s="15"/>
       <c r="AR71" s="15"/>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A72" s="8" t="s">
-        <v>83</v>
-      </c>
+    <row r="72" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
       <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
+      <c r="C72" s="9" t="s">
+        <v>95</v>
+      </c>
       <c r="D72" s="10"/>
-      <c r="E72" s="10"/>
+      <c r="E72" s="10">
+        <v>3</v>
+      </c>
       <c r="F72" s="11">
-        <v>43048</v>
+        <v>43206</v>
       </c>
       <c r="G72" s="11">
-        <v>43048</v>
+        <v>43206</v>
       </c>
       <c r="H72" s="11">
-        <v>43190</v>
-      </c>
-      <c r="I72" s="11">
-        <v>43190</v>
-      </c>
-      <c r="J72" s="33"/>
-      <c r="K72" s="14"/>
+        <v>43217</v>
+      </c>
+      <c r="I72" s="12"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="L72" s="15"/>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
@@ -5399,8 +5406,8 @@
       <c r="U72" s="15"/>
       <c r="V72" s="15"/>
       <c r="W72" s="15"/>
-      <c r="X72" s="28"/>
-      <c r="Y72" s="28"/>
+      <c r="X72" s="15"/>
+      <c r="Y72" s="15"/>
       <c r="Z72" s="15"/>
       <c r="AA72" s="15"/>
       <c r="AB72" s="15"/>
@@ -5421,33 +5428,29 @@
       <c r="AQ72" s="15"/>
       <c r="AR72" s="15"/>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:44" outlineLevel="2" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
-      <c r="B73" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="18" t="s">
+        <v>96</v>
+      </c>
       <c r="D73" s="10"/>
       <c r="E73" s="10">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F73" s="11">
-        <v>43048</v>
+        <v>43206</v>
       </c>
       <c r="G73" s="11">
-        <v>43048</v>
+        <v>43206</v>
       </c>
       <c r="H73" s="11">
-        <v>43051</v>
-      </c>
-      <c r="I73" s="11">
-        <v>43051</v>
-      </c>
-      <c r="J73" s="17">
-        <v>1</v>
-      </c>
-      <c r="K73" s="14" t="s">
-        <v>33</v>
+        <v>43217</v>
+      </c>
+      <c r="I73" s="12"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="L73" s="15"/>
       <c r="M73" s="15"/>
@@ -5461,8 +5464,8 @@
       <c r="U73" s="15"/>
       <c r="V73" s="15"/>
       <c r="W73" s="15"/>
-      <c r="X73" s="28"/>
-      <c r="Y73" s="29"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
       <c r="Z73" s="15"/>
       <c r="AA73" s="15"/>
       <c r="AB73" s="15"/>
@@ -5483,33 +5486,33 @@
       <c r="AQ73" s="15"/>
       <c r="AR73" s="15"/>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A74" s="8"/>
-      <c r="B74" s="9" t="s">
-        <v>88</v>
-      </c>
+    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" s="9"/>
       <c r="C74" s="9"/>
       <c r="D74" s="10"/>
       <c r="E74" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F74" s="11">
-        <v>43185</v>
+        <v>43199</v>
       </c>
       <c r="G74" s="11">
-        <v>43185</v>
+        <v>43199</v>
       </c>
       <c r="H74" s="11">
-        <v>43190</v>
+        <v>43203</v>
       </c>
       <c r="I74" s="11">
-        <v>43190</v>
+        <v>43202</v>
       </c>
       <c r="J74" s="17">
         <v>1</v>
       </c>
       <c r="K74" s="14" t="s">
-        <v>97</v>
+        <v>19</v>
       </c>
       <c r="L74" s="15"/>
       <c r="M74" s="15"/>
@@ -5521,10 +5524,10 @@
       <c r="S74" s="15"/>
       <c r="T74" s="15"/>
       <c r="U74" s="15"/>
-      <c r="V74" s="15"/>
+      <c r="V74" s="29"/>
       <c r="W74" s="15"/>
-      <c r="X74" s="28"/>
-      <c r="Y74" s="28"/>
+      <c r="X74" s="15"/>
+      <c r="Y74" s="15"/>
       <c r="Z74" s="15"/>
       <c r="AA74" s="15"/>
       <c r="AB74" s="15"/>
@@ -5539,19 +5542,199 @@
       <c r="AK74" s="15"/>
       <c r="AL74" s="15"/>
       <c r="AM74" s="15"/>
-      <c r="AN74" s="29"/>
+      <c r="AN74" s="15"/>
       <c r="AO74" s="15"/>
       <c r="AP74" s="15"/>
       <c r="AQ74" s="15"/>
       <c r="AR74" s="15"/>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="D75" s="36" t="s">
+    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A75" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="11">
+        <v>43048</v>
+      </c>
+      <c r="G75" s="11">
+        <v>43048</v>
+      </c>
+      <c r="H75" s="11">
+        <v>43190</v>
+      </c>
+      <c r="I75" s="11">
+        <v>43190</v>
+      </c>
+      <c r="J75" s="33"/>
+      <c r="K75" s="14"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15"/>
+      <c r="U75" s="15"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="15"/>
+      <c r="X75" s="28"/>
+      <c r="Y75" s="28"/>
+      <c r="Z75" s="15"/>
+      <c r="AA75" s="15"/>
+      <c r="AB75" s="15"/>
+      <c r="AC75" s="15"/>
+      <c r="AD75" s="15"/>
+      <c r="AE75" s="15"/>
+      <c r="AF75" s="15"/>
+      <c r="AG75" s="15"/>
+      <c r="AH75" s="15"/>
+      <c r="AI75" s="15"/>
+      <c r="AJ75" s="15"/>
+      <c r="AK75" s="15"/>
+      <c r="AL75" s="15"/>
+      <c r="AM75" s="15"/>
+      <c r="AN75" s="15"/>
+      <c r="AO75" s="15"/>
+      <c r="AP75" s="15"/>
+      <c r="AQ75" s="15"/>
+      <c r="AR75" s="15"/>
+    </row>
+    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A76" s="8"/>
+      <c r="B76" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E75" s="35">
-        <f>SUM(E3:E74)</f>
-        <v>195</v>
+      <c r="C76" s="9"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10">
+        <v>20</v>
+      </c>
+      <c r="F76" s="11">
+        <v>43048</v>
+      </c>
+      <c r="G76" s="11">
+        <v>43048</v>
+      </c>
+      <c r="H76" s="11">
+        <v>43051</v>
+      </c>
+      <c r="I76" s="11">
+        <v>43051</v>
+      </c>
+      <c r="J76" s="17">
+        <v>1</v>
+      </c>
+      <c r="K76" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+      <c r="T76" s="15"/>
+      <c r="U76" s="15"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="15"/>
+      <c r="X76" s="28"/>
+      <c r="Y76" s="29"/>
+      <c r="Z76" s="15"/>
+      <c r="AA76" s="15"/>
+      <c r="AB76" s="15"/>
+      <c r="AC76" s="15"/>
+      <c r="AD76" s="15"/>
+      <c r="AE76" s="15"/>
+      <c r="AF76" s="15"/>
+      <c r="AG76" s="15"/>
+      <c r="AH76" s="15"/>
+      <c r="AI76" s="15"/>
+      <c r="AJ76" s="15"/>
+      <c r="AK76" s="15"/>
+      <c r="AL76" s="15"/>
+      <c r="AM76" s="15"/>
+      <c r="AN76" s="15"/>
+      <c r="AO76" s="15"/>
+      <c r="AP76" s="15"/>
+      <c r="AQ76" s="15"/>
+      <c r="AR76" s="15"/>
+    </row>
+    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="A77" s="8"/>
+      <c r="B77" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10">
+        <v>4</v>
+      </c>
+      <c r="F77" s="11">
+        <v>43185</v>
+      </c>
+      <c r="G77" s="11">
+        <v>43185</v>
+      </c>
+      <c r="H77" s="11">
+        <v>43190</v>
+      </c>
+      <c r="I77" s="11">
+        <v>43190</v>
+      </c>
+      <c r="J77" s="17">
+        <v>1</v>
+      </c>
+      <c r="K77" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+      <c r="T77" s="15"/>
+      <c r="U77" s="15"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="15"/>
+      <c r="X77" s="28"/>
+      <c r="Y77" s="28"/>
+      <c r="Z77" s="15"/>
+      <c r="AA77" s="15"/>
+      <c r="AB77" s="15"/>
+      <c r="AC77" s="15"/>
+      <c r="AD77" s="15"/>
+      <c r="AE77" s="15"/>
+      <c r="AF77" s="15"/>
+      <c r="AG77" s="15"/>
+      <c r="AH77" s="15"/>
+      <c r="AI77" s="15"/>
+      <c r="AJ77" s="15"/>
+      <c r="AK77" s="15"/>
+      <c r="AL77" s="15"/>
+      <c r="AM77" s="15"/>
+      <c r="AN77" s="29"/>
+      <c r="AO77" s="15"/>
+      <c r="AP77" s="15"/>
+      <c r="AQ77" s="15"/>
+      <c r="AR77" s="15"/>
+    </row>
+    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="D78" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="E78" s="35">
+        <f>SUM(E3:E77)</f>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>